<commit_message>
added a downloading page
</commit_message>
<xml_diff>
--- a/xlsx/filtered_songs.xlsx
+++ b/xlsx/filtered_songs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,13 +424,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">Tui Hobi Amar Bohu Purulia Romantic Song Kundan Kumar.mp3 </v>
+        <v xml:space="preserve">Sundori Ruposhi Jagdish nd Priyanka New Purulia Romantic Songs Download.mp3 </v>
       </c>
       <c r="B2" t="str">
-        <v>https://puruliadj.in/download/780/tui_hobi_amar_bohu_purulia_romantic_song_kundan_kumar</v>
+        <v>https://puruliadj.in/download/924/sundori_ruposhi_jagdish_nd_priyanka_new_purulia_romantic_songs_download</v>
       </c>
       <c r="C2" t="str">
-        <v>https://puruliadj.in/files/download/id/780</v>
+        <v>https://puruliadj.in/files/download/id/924</v>
       </c>
       <c r="D2" t="str">
         <v>(New Purulia Songs)</v>
@@ -444,13 +444,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">A Khapi Tui Amar Jiwan New Purulia Romantic Song Singer- Manoj Das Mira Das.mp3 </v>
+        <v xml:space="preserve">Dukho Ektai Dukho Shankar Tantubai and Mira Das New Purulia Song.mp3 </v>
       </c>
       <c r="B3" t="str">
-        <v>https://puruliadj.in/download/779/a_khapi_tui_amar_jiwan_new_purulia_romantic_song_singer-_manoj_das_mira_das</v>
+        <v>https://puruliadj.in/download/910/dukho_ektai_dukho_shankar_tantubai_and_mira_das_new_purulia_song</v>
       </c>
       <c r="C3" t="str">
-        <v>https://puruliadj.in/files/download/id/779</v>
+        <v>https://puruliadj.in/files/download/id/910</v>
       </c>
       <c r="D3" t="str">
         <v>(New Purulia Songs)</v>
@@ -464,19 +464,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">Tui Sona Sukhe Aachis Aamake Chhare Jagdish Kumar Purulia Hits Songs.mp3 </v>
+        <v xml:space="preserve">Dada Re Ka Amai Dakba Bon Bale Bidai Geet Kanika Karmakar New Purulia Song 2024.mp3 </v>
       </c>
       <c r="B4" t="str">
-        <v>https://puruliadj.in/download/775/tui_sona_sukhe_aachis_aamake_chhare_jagdish_kumar_purulia_hits_songs</v>
+        <v>https://puruliadj.in/download/904/dada_re_ka_amai_dakba_bon_bale_bidai_geet_kanika_karmakar_new_purulia_song_2024</v>
       </c>
       <c r="C4" t="str">
-        <v>https://puruliadj.in/files/download/id/775</v>
+        <v>https://puruliadj.in/files/download/id/904</v>
       </c>
       <c r="D4" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E4" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Kanika Karmakar - Bihar Gann Purulia Songs</v>
       </c>
       <c r="F4" t="str">
         <v>class</v>
@@ -484,13 +484,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v xml:space="preserve">Tui To Chili Amar Jiboner Jibon New Purulia Mp3 Song Singer - Karno Kumar.mp3 </v>
+        <v xml:space="preserve">Sopner Rani - Raja New Purulia Romantic Song Singer Manoj Das Smritikona Roy.mp3 </v>
       </c>
       <c r="B5" t="str">
-        <v>https://puruliadj.in/download/774/tui_to_chili_amar_jiboner_jibon_new_purulia_mp3_song_singer_-_karno_kumar</v>
+        <v>https://puruliadj.in/download/898/sopner_rani_-_raja_new_purulia_romantic_song_singer_manoj_das_smritikona_roy</v>
       </c>
       <c r="C5" t="str">
-        <v>https://puruliadj.in/files/download/id/774</v>
+        <v>https://puruliadj.in/files/download/id/898</v>
       </c>
       <c r="D5" t="str">
         <v>(New Purulia Songs)</v>
@@ -499,58 +499,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F5" t="str">
-        <v>10.74 mb</v>
+        <v>8.61 mb</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v xml:space="preserve">Ai Buka a Paing Hila Jacha Re Jagdish Kajal New Purulia Song Romantic Love.mp3 </v>
+        <v xml:space="preserve">Duniya Soble Boro Mayo Ar Bapo Go Chumki Rani Bihar Gann Kudmali Bihar Geet.mp3 </v>
       </c>
       <c r="B6" t="str">
-        <v>https://puruliadj.in/download/773/ai_buka_a_paing_hila_jacha_re_jagdish_kajal_new_purulia_song_romantic_love</v>
+        <v>https://puruliadj.in/download/833/duniya_soble_boro_mayo_ar_bapo_go_chumki_rani_bihar_gann_kudmali_bihar_geet</v>
       </c>
       <c r="C6" t="str">
-        <v>https://puruliadj.in/files/download/id/773</v>
+        <v>https://puruliadj.in/files/download/id/833</v>
       </c>
       <c r="D6" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E6" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Chumki Rani Mahato Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F6" t="str">
-        <v>8.73 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v xml:space="preserve">Torei Rupe Ami Pagol Superhit Jhumur Song Goutam Mohanta.mp3 </v>
+        <v xml:space="preserve">Cycle Dili Ghori Dili Kudmali Bihar Geet Bihar Gaan Jhumur Song Tapati Mahato.mp3 </v>
       </c>
       <c r="B7" t="str">
-        <v>https://puruliadj.in/download/733/torei_rupe_ami_pagol_superhit_jhumur_song_goutam_mohanta</v>
+        <v>https://puruliadj.in/download/832/cycle_dili_ghori_dili_kudmali_bihar_geet_bihar_gaan_jhumur_song_tapati_mahato</v>
       </c>
       <c r="C7" t="str">
-        <v>https://puruliadj.in/files/download/id/733</v>
+        <v>https://puruliadj.in/files/download/id/832</v>
       </c>
       <c r="D7" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E7" t="str">
-        <v>Popular Jhumur Songs</v>
+        <v>Tapati Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F7" t="str">
-        <v>9.08 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v xml:space="preserve">Shwapne Dekhi Mon Pakhi Shankar Tantubai Mira Das Purulia New Song.mp3 </v>
+        <v xml:space="preserve">Thokbaj Romantic Bewafa Purulia Sad Song Singer - Raju Sahis New Attitude Sad Song.mp3 </v>
       </c>
       <c r="B8" t="str">
-        <v>https://puruliadj.in/download/728/shwapne_dekhi_mon_pakhi_shankar_tantubai_mira_das_purulia_new_song</v>
+        <v>https://puruliadj.in/download/825/thokbaj_romantic_bewafa_purulia_sad_song_singer_-_raju_sahis_new_attitude_sad_song</v>
       </c>
       <c r="C8" t="str">
-        <v>https://puruliadj.in/files/download/id/728</v>
+        <v>https://puruliadj.in/files/download/id/825</v>
       </c>
       <c r="D8" t="str">
         <v>(New Purulia Songs)</v>
@@ -559,24 +559,24 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F8" t="str">
-        <v>class</v>
+        <v>9.26 mb</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v xml:space="preserve">O Jamai Babu Baran Karo Bihar Geet Anjali Mahata Jhumur Song Jhargram Jhumur.mp3 </v>
+        <v xml:space="preserve">Param Sundari Singer - Pinki Mahata New Jhargram Jhumur Song.mp3 </v>
       </c>
       <c r="B9" t="str">
-        <v>https://puruliadj.in/download/725/o_jamai_babu_baran_karo_bihar_geet_anjali_mahata_jhumur_song_jhargram_jhumur</v>
+        <v>https://puruliadj.in/download/823/param_sundari_singer_-_pinki_mahata_new_jhargram_jhumur_song</v>
       </c>
       <c r="C9" t="str">
-        <v>https://puruliadj.in/files/download/id/725</v>
+        <v>https://puruliadj.in/files/download/id/823</v>
       </c>
       <c r="D9" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E9" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F9" t="str">
         <v>class</v>
@@ -584,19 +584,19 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v xml:space="preserve">Babai Valo Baise Chilo Anjali Mahata Bangla Jhumur  Biha Geet Jhargram jhumur Song.mp3 </v>
+        <v xml:space="preserve">Tui Hobi Amar Bohu Purulia Romantic Song Kundan Kumar.mp3 </v>
       </c>
       <c r="B10" t="str">
-        <v>https://puruliadj.in/download/718/babai_valo_baise_chilo_anjali_mahata_bangla_jhumur__biha_geet_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/780/tui_hobi_amar_bohu_purulia_romantic_song_kundan_kumar</v>
       </c>
       <c r="C10" t="str">
-        <v>https://puruliadj.in/files/download/id/718</v>
+        <v>https://puruliadj.in/files/download/id/780</v>
       </c>
       <c r="D10" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E10" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F10" t="str">
         <v>class</v>
@@ -604,19 +604,19 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v xml:space="preserve">Koto Dure Acha Baba Anjali Mahata Biha Ghor Geet Jhargram Jhumur.mp3 </v>
+        <v xml:space="preserve">A Khapi Tui Amar Jiwan New Purulia Romantic Song Singer- Manoj Das Mira Das.mp3 </v>
       </c>
       <c r="B11" t="str">
-        <v>https://puruliadj.in/download/717/koto_dure_acha_baba_anjali_mahata_biha_ghor_geet_jhargram_jhumur</v>
+        <v>https://puruliadj.in/download/779/a_khapi_tui_amar_jiwan_new_purulia_romantic_song_singer-_manoj_das_mira_das</v>
       </c>
       <c r="C11" t="str">
-        <v>https://puruliadj.in/files/download/id/717</v>
+        <v>https://puruliadj.in/files/download/id/779</v>
       </c>
       <c r="D11" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E11" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F11" t="str">
         <v>class</v>
@@ -624,19 +624,19 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v xml:space="preserve">Amm Dale Mahul Dale Bihar Geet Jhumur Song Anjali Mahato Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Tui Sona Sukhe Aachis Aamake Chhare Jagdish Kumar Purulia Hits Songs.mp3 </v>
       </c>
       <c r="B12" t="str">
-        <v>https://puruliadj.in/download/716/amm_dale_mahul_dale_bihar_geet_jhumur_song_anjali_mahato_jhumur_song</v>
+        <v>https://puruliadj.in/download/775/tui_sona_sukhe_aachis_aamake_chhare_jagdish_kumar_purulia_hits_songs</v>
       </c>
       <c r="C12" t="str">
-        <v>https://puruliadj.in/files/download/id/716</v>
+        <v>https://puruliadj.in/files/download/id/775</v>
       </c>
       <c r="D12" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E12" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F12" t="str">
         <v>class</v>
@@ -644,99 +644,99 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v xml:space="preserve">Beha Korte Jabek Bor Babu Biha ghor Anjali Mahato Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Tui To Chili Amar Jiboner Jibon New Purulia Mp3 Song Singer - Karno Kumar.mp3 </v>
       </c>
       <c r="B13" t="str">
-        <v>https://puruliadj.in/download/715/beha_korte_jabek_bor_babu_biha_ghor_anjali_mahato_jhumur_song</v>
+        <v>https://puruliadj.in/download/774/tui_to_chili_amar_jiboner_jibon_new_purulia_mp3_song_singer_-_karno_kumar</v>
       </c>
       <c r="C13" t="str">
-        <v>https://puruliadj.in/files/download/id/715</v>
+        <v>https://puruliadj.in/files/download/id/774</v>
       </c>
       <c r="D13" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E13" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F13" t="str">
-        <v>class</v>
+        <v>10.74 mb</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v xml:space="preserve">Eto Din Ja Rakhli Mai Go Bihar Geet Volume 1 Anjali Mahata Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Ai Buka a Paing Hila Jacha Re Jagdish Kajal New Purulia Song Romantic Love.mp3 </v>
       </c>
       <c r="B14" t="str">
-        <v>https://puruliadj.in/download/714/eto_din_ja_rakhli_mai_go_bihar_geet_volume_1_anjali_mahata_jhumur_song</v>
+        <v>https://puruliadj.in/download/773/ai_buka_a_paing_hila_jacha_re_jagdish_kajal_new_purulia_song_romantic_love</v>
       </c>
       <c r="C14" t="str">
-        <v>https://puruliadj.in/files/download/id/714</v>
+        <v>https://puruliadj.in/files/download/id/773</v>
       </c>
       <c r="D14" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E14" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F14" t="str">
-        <v>13.2 mb</v>
+        <v>8.73 mb</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v xml:space="preserve">Biha Ghore Bajbajna Keo Hase Bihar Geet Anjali Mahato Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Torei Rupe Ami Pagol Superhit Jhumur Song Goutam Mohanta.mp3 </v>
       </c>
       <c r="B15" t="str">
-        <v>https://puruliadj.in/download/713/biha_ghore_bajbajna_keo_hase_bihar_geet_anjali_mahato_jhumur_song</v>
+        <v>https://puruliadj.in/download/733/torei_rupe_ami_pagol_superhit_jhumur_song_goutam_mohanta</v>
       </c>
       <c r="C15" t="str">
-        <v>https://puruliadj.in/files/download/id/713</v>
+        <v>https://puruliadj.in/files/download/id/733</v>
       </c>
       <c r="D15" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E15" t="str">
-        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
+        <v>Popular Jhumur Songs</v>
       </c>
       <c r="F15" t="str">
-        <v>class</v>
+        <v>9.08 mb</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v xml:space="preserve">Koina Dekhate Asilo Jhaken New Jhumur Song Singer Sonali Mahata.mp3.mp3 </v>
+        <v xml:space="preserve">Shwapne Dekhi Mon Pakhi Shankar Tantubai Mira Das Purulia New Song.mp3 </v>
       </c>
       <c r="B16" t="str">
-        <v>https://puruliadj.in/download/709/koina_dekhate_asilo_jhaken_new_jhumur_song_singer_sonali_mahata</v>
+        <v>https://puruliadj.in/download/728/shwapne_dekhi_mon_pakhi_shankar_tantubai_mira_das_purulia_new_song</v>
       </c>
       <c r="C16" t="str">
-        <v>https://puruliadj.in/files/download/id/709</v>
+        <v>https://puruliadj.in/files/download/id/728</v>
       </c>
       <c r="D16" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E16" t="str">
-        <v>New Kurmali Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F16" t="str">
-        <v>7.9 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v xml:space="preserve">Tor Opekhai Jagadish New Purulia Mp3 Songs Download.mp3 </v>
+        <v xml:space="preserve">O Jamai Babu Baran Karo Bihar Geet Anjali Mahata Jhumur Song Jhargram Jhumur.mp3 </v>
       </c>
       <c r="B17" t="str">
-        <v>https://puruliadj.in/download/704/tor_opekhai_jagadish_new_purulia_mp3_songs_download</v>
+        <v>https://puruliadj.in/download/725/o_jamai_babu_baran_karo_bihar_geet_anjali_mahata_jhumur_song_jhargram_jhumur</v>
       </c>
       <c r="C17" t="str">
-        <v>https://puruliadj.in/files/download/id/704</v>
+        <v>https://puruliadj.in/files/download/id/725</v>
       </c>
       <c r="D17" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E17" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F17" t="str">
         <v>class</v>
@@ -744,19 +744,19 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v xml:space="preserve">Kar Kotha Sune Amar Mon Kandali Singer Karna Kumar nd Mira Das.mp3 </v>
+        <v xml:space="preserve">Babai Valo Baise Chilo Anjali Mahata Bangla Jhumur  Biha Geet Jhargram jhumur Song.mp3 </v>
       </c>
       <c r="B18" t="str">
-        <v>https://puruliadj.in/download/700/kar_kotha_sune_amar_mon_kandali_singer_karna_kumar_nd_mira_das</v>
+        <v>https://puruliadj.in/download/718/babai_valo_baise_chilo_anjali_mahata_bangla_jhumur__biha_geet_jhargram_jhumur_song</v>
       </c>
       <c r="C18" t="str">
-        <v>https://puruliadj.in/files/download/id/700</v>
+        <v>https://puruliadj.in/files/download/id/718</v>
       </c>
       <c r="D18" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E18" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F18" t="str">
         <v>class</v>
@@ -764,159 +764,159 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v xml:space="preserve">Sal Baner Kurkut New Jhumar Song Singer Kiran Mohanta Kurmali Song.mp3 </v>
+        <v xml:space="preserve">Koto Dure Acha Baba Anjali Mahata Biha Ghor Geet Jhargram Jhumur.mp3 </v>
       </c>
       <c r="B19" t="str">
-        <v>https://puruliadj.in/download/694/sal_baner_kurkut_new_jhumar_song_singer_kiran_mohanta_kurmali_song</v>
+        <v>https://puruliadj.in/download/717/koto_dure_acha_baba_anjali_mahata_biha_ghor_geet_jhargram_jhumur</v>
       </c>
       <c r="C19" t="str">
-        <v>https://puruliadj.in/files/download/id/694</v>
+        <v>https://puruliadj.in/files/download/id/717</v>
       </c>
       <c r="D19" t="str">
         <v>(All Festivals Songs)</v>
       </c>
       <c r="E19" t="str">
-        <v>New Kurmali Jhumur Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F19" t="str">
-        <v>11.44 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v xml:space="preserve">Mon Ta Niya Cheli Hase Hase New Purulia Song Singer - Kundan Kumar.mp3 </v>
+        <v xml:space="preserve">Amm Dale Mahul Dale Bihar Geet Jhumur Song Anjali Mahato Jhumur Song.mp3 </v>
       </c>
       <c r="B20" t="str">
-        <v>https://puruliadj.in/download/693/mon_ta_niya_cheli_hase_hase_new_purulia_song_singer_-_kundan_kumar</v>
+        <v>https://puruliadj.in/download/716/amm_dale_mahul_dale_bihar_geet_jhumur_song_anjali_mahato_jhumur_song</v>
       </c>
       <c r="C20" t="str">
-        <v>https://puruliadj.in/files/download/id/693</v>
+        <v>https://puruliadj.in/files/download/id/716</v>
       </c>
       <c r="D20" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E20" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F20" t="str">
-        <v>9.86 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v xml:space="preserve">Lagilo Mone Agun New Purulia Gan Romantic Song Singar - Usha Rani.mp3 </v>
+        <v xml:space="preserve">Beha Korte Jabek Bor Babu Biha ghor Anjali Mahato Jhumur Song.mp3 </v>
       </c>
       <c r="B21" t="str">
-        <v>https://puruliadj.in/download/692/lagilo_mone_agun_new_purulia_gan_romantic_song_singar_-_usha_rani</v>
+        <v>https://puruliadj.in/download/715/beha_korte_jabek_bor_babu_biha_ghor_anjali_mahato_jhumur_song</v>
       </c>
       <c r="C21" t="str">
-        <v>https://puruliadj.in/files/download/id/692</v>
+        <v>https://puruliadj.in/files/download/id/715</v>
       </c>
       <c r="D21" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E21" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F21" t="str">
-        <v>8.01 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v xml:space="preserve">Baimani Sona Bewafa Sad Song New Purulia Gann - Jagadish Kumar.mp3 </v>
+        <v xml:space="preserve">Eto Din Ja Rakhli Mai Go Bihar Geet Volume 1 Anjali Mahata Jhumur Song.mp3 </v>
       </c>
       <c r="B22" t="str">
-        <v>https://puruliadj.in/download/690/baimani_sona_bewafa_sad_song_new_purulia_gann_-_jagadish_kumar</v>
+        <v>https://puruliadj.in/download/714/eto_din_ja_rakhli_mai_go_bihar_geet_volume_1_anjali_mahata_jhumur_song</v>
       </c>
       <c r="C22" t="str">
-        <v>https://puruliadj.in/files/download/id/690</v>
+        <v>https://puruliadj.in/files/download/id/714</v>
       </c>
       <c r="D22" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E22" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F22" t="str">
-        <v>8.66 mb</v>
+        <v>13.2 mb</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v xml:space="preserve">Thokali Amake Beiman Tui Pasani Kundan Kumar New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Biha Ghore Bajbajna Keo Hase Bihar Geet Anjali Mahato Jhumur Song.mp3 </v>
       </c>
       <c r="B23" t="str">
-        <v>https://puruliadj.in/download/689/thokali_amake_beiman_tui_pasani_kundan_kumar_new_purulia_song</v>
+        <v>https://puruliadj.in/download/713/biha_ghore_bajbajna_keo_hase_bihar_geet_anjali_mahato_jhumur_song</v>
       </c>
       <c r="C23" t="str">
-        <v>https://puruliadj.in/files/download/id/689</v>
+        <v>https://puruliadj.in/files/download/id/713</v>
       </c>
       <c r="D23" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E23" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Anjali Mahata Bihar Geet Jhumur Songs</v>
       </c>
       <c r="F23" t="str">
-        <v>8.12 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v xml:space="preserve">Hai Re Ghayel Hour Gelo Chengla Chela Mira Das New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Koina Dekhate Asilo Jhaken New Jhumur Song Singer Sonali Mahata.mp3.mp3 </v>
       </c>
       <c r="B24" t="str">
-        <v>https://puruliadj.in/download/675/hai_re_ghayel_hour_gelo_chengla_chela_mira_das_new_purulia_song</v>
+        <v>https://puruliadj.in/download/709/koina_dekhate_asilo_jhaken_new_jhumur_song_singer_sonali_mahata</v>
       </c>
       <c r="C24" t="str">
-        <v>https://puruliadj.in/files/download/id/675</v>
+        <v>https://puruliadj.in/files/download/id/709</v>
       </c>
       <c r="D24" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E24" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Kurmali Jhumur Songs</v>
       </c>
       <c r="F24" t="str">
-        <v>class</v>
+        <v>7.9 mb</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v xml:space="preserve">Mon Bole Bhalobasha Kare Le Paritosh Mahata Pratima Mahata New Song.mp3 </v>
+        <v xml:space="preserve">Tor Opekhai Jagadish New Purulia Mp3 Songs Download.mp3 </v>
       </c>
       <c r="B25" t="str">
-        <v>https://puruliadj.in/download/674/mon_bole_bhalobasha_kare_le_paritosh_mahata_pratima_mahata_new_song</v>
+        <v>https://puruliadj.in/download/704/tor_opekhai_jagadish_new_purulia_mp3_songs_download</v>
       </c>
       <c r="C25" t="str">
-        <v>https://puruliadj.in/files/download/id/674</v>
+        <v>https://puruliadj.in/files/download/id/704</v>
       </c>
       <c r="D25" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E25" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F25" t="str">
-        <v>7.05 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v xml:space="preserve">Golap Full Tor Hata Dhorai Diba Re Pratima Mahata Kundan Kumar New Song.mp3 </v>
+        <v xml:space="preserve">Kar Kotha Sune Amar Mon Kandali Singer Karna Kumar nd Mira Das.mp3 </v>
       </c>
       <c r="B26" t="str">
-        <v>https://puruliadj.in/download/673/golap_full_tor_hata_dhorai_diba_re_pratima_mahata_kundan_kumar_new_song</v>
+        <v>https://puruliadj.in/download/700/kar_kotha_sune_amar_mon_kandali_singer_karna_kumar_nd_mira_das</v>
       </c>
       <c r="C26" t="str">
-        <v>https://puruliadj.in/files/download/id/673</v>
+        <v>https://puruliadj.in/files/download/id/700</v>
       </c>
       <c r="D26" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E26" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F26" t="str">
         <v>class</v>
@@ -924,119 +924,119 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v xml:space="preserve">Ami Kuwara Tui Kuwari New Jhargram Purulia Modern Song Purulia Romantic Song.mp3 </v>
+        <v xml:space="preserve">Sal Baner Kurkut New Jhumar Song Singer Kiran Mohanta Kurmali Song.mp3 </v>
       </c>
       <c r="B27" t="str">
-        <v>https://puruliadj.in/download/664/ami_kuwara_tui_kuwari_new_jhargram_purulia_modern_song_purulia_romantic_song</v>
+        <v>https://puruliadj.in/download/694/sal_baner_kurkut_new_jhumar_song_singer_kiran_mohanta_kurmali_song</v>
       </c>
       <c r="C27" t="str">
-        <v>https://puruliadj.in/files/download/id/664</v>
+        <v>https://puruliadj.in/files/download/id/694</v>
       </c>
       <c r="D27" t="str">
         <v>(All Festivals Songs)</v>
       </c>
       <c r="E27" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Kurmali Jhumur Songs</v>
       </c>
       <c r="F27" t="str">
-        <v>5.64 mb</v>
+        <v>11.44 mb</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v xml:space="preserve">Chamra Tolai Nachbo Dujon Bihar Dine Piu Rani Mahato New Purulia Jhargram New Song.mp3 </v>
+        <v xml:space="preserve">Mon Ta Niya Cheli Hase Hase New Purulia Song Singer - Kundan Kumar.mp3 </v>
       </c>
       <c r="B28" t="str">
-        <v>https://puruliadj.in/download/662/chamra_tolai_nachbo_dujon_bihar_dine_piu_rani_mahato_new_purulia_jhargram_new_song</v>
+        <v>https://puruliadj.in/download/693/mon_ta_niya_cheli_hase_hase_new_purulia_song_singer_-_kundan_kumar</v>
       </c>
       <c r="C28" t="str">
-        <v>https://puruliadj.in/files/download/id/662</v>
+        <v>https://puruliadj.in/files/download/id/693</v>
       </c>
       <c r="D28" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E28" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F28" t="str">
-        <v>class</v>
+        <v>9.86 mb</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v xml:space="preserve">Cholka Cholka Pare Jacha Amar Kakher Kalshi Singer - AJ Lipini New Jhargram Purulia Song.mp3 </v>
+        <v xml:space="preserve">Lagilo Mone Agun New Purulia Gan Romantic Song Singar - Usha Rani.mp3 </v>
       </c>
       <c r="B29" t="str">
-        <v>https://puruliadj.in/download/657/cholka_cholka_pare_jacha_amar_kakher_kalshi_singer_-_aj_lipini_new_jhargram_purulia_song</v>
+        <v>https://puruliadj.in/download/692/lagilo_mone_agun_new_purulia_gan_romantic_song_singar_-_usha_rani</v>
       </c>
       <c r="C29" t="str">
-        <v>https://puruliadj.in/files/download/id/657</v>
+        <v>https://puruliadj.in/files/download/id/692</v>
       </c>
       <c r="D29" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E29" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F29" t="str">
-        <v>5.07 mb</v>
+        <v>8.01 mb</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v xml:space="preserve">Tor Bihar Pendal Ami Bonaichi Singer - Poritosh nd AJ Lipini  New Purulia Sed Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Baimani Sona Bewafa Sad Song New Purulia Gann - Jagadish Kumar.mp3 </v>
       </c>
       <c r="B30" t="str">
-        <v>https://puruliadj.in/download/656/tor_bihar_pendal_ami_bonaichi_singer_-_poritosh_nd_aj_lipini__new_purulia_sed_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/690/baimani_sona_bewafa_sad_song_new_purulia_gann_-_jagadish_kumar</v>
       </c>
       <c r="C30" t="str">
-        <v>https://puruliadj.in/files/download/id/656</v>
+        <v>https://puruliadj.in/files/download/id/690</v>
       </c>
       <c r="D30" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E30" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F30" t="str">
-        <v>8.85 mb</v>
+        <v>8.66 mb</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v xml:space="preserve">Lukai Lukai Kandis Na Valoi hobe tor bor Singer - Paritosh Mahata AJ Lipini.mp3 </v>
+        <v xml:space="preserve">Thokali Amake Beiman Tui Pasani Kundan Kumar New Purulia Song.mp3 </v>
       </c>
       <c r="B31" t="str">
-        <v>https://puruliadj.in/download/655/lukai_lukai_kandis_na_valoi_hobe_tor_bor_singer_-_paritosh_mahata_aj_lipini</v>
+        <v>https://puruliadj.in/download/689/thokali_amake_beiman_tui_pasani_kundan_kumar_new_purulia_song</v>
       </c>
       <c r="C31" t="str">
-        <v>https://puruliadj.in/files/download/id/655</v>
+        <v>https://puruliadj.in/files/download/id/689</v>
       </c>
       <c r="D31" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E31" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F31" t="str">
-        <v>class</v>
+        <v>8.12 mb</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v xml:space="preserve">Ghagra Bali Re Perit Hoye Jaba Singer - Kumar Paritosh Mahata New Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Hai Re Ghayel Hour Gelo Chengla Chela Mira Das New Purulia Song.mp3 </v>
       </c>
       <c r="B32" t="str">
-        <v>https://puruliadj.in/download/654/ghagra_bali_re_perit_hoye_jaba_singer_-_kumar_paritosh_mahata_new_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/675/hai_re_ghayel_hour_gelo_chengla_chela_mira_das_new_purulia_song</v>
       </c>
       <c r="C32" t="str">
-        <v>https://puruliadj.in/files/download/id/654</v>
+        <v>https://puruliadj.in/files/download/id/675</v>
       </c>
       <c r="D32" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E32" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F32" t="str">
         <v>class</v>
@@ -1044,39 +1044,39 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v xml:space="preserve">Ai Dekhe Ja Purulia Jhargram Bakura Singer - Purnima Mandi New Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Mon Bole Bhalobasha Kare Le Paritosh Mahata Pratima Mahata New Song.mp3 </v>
       </c>
       <c r="B33" t="str">
-        <v>https://puruliadj.in/download/652/ai_dekhe_ja_purulia_jhargram_bakura_singer_-_purnima_mandi_new_jhumur_song</v>
+        <v>https://puruliadj.in/download/674/mon_bole_bhalobasha_kare_le_paritosh_mahata_pratima_mahata_new_song</v>
       </c>
       <c r="C33" t="str">
-        <v>https://puruliadj.in/files/download/id/652</v>
+        <v>https://puruliadj.in/files/download/id/674</v>
       </c>
       <c r="D33" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E33" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F33" t="str">
-        <v>class</v>
+        <v>7.05 mb</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v xml:space="preserve">Young Bandhu Dharo Hat Singer - Purnima Mandi New Jhumur Song - Download.mp3 </v>
+        <v xml:space="preserve">Golap Full Tor Hata Dhorai Diba Re Pratima Mahata Kundan Kumar New Song.mp3 </v>
       </c>
       <c r="B34" t="str">
-        <v>https://puruliadj.in/download/651/young_bandhu_dharo_hat_singer_-_purnima_mandi_new_jhumur_song_-_download</v>
+        <v>https://puruliadj.in/download/673/golap_full_tor_hata_dhorai_diba_re_pratima_mahata_kundan_kumar_new_song</v>
       </c>
       <c r="C34" t="str">
-        <v>https://puruliadj.in/files/download/id/651</v>
+        <v>https://puruliadj.in/files/download/id/673</v>
       </c>
       <c r="D34" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E34" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F34" t="str">
         <v>class</v>
@@ -1084,39 +1084,39 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v xml:space="preserve">Purnimar Bhalobasha Singer - Purnima Mandi New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Ami Kuwara Tui Kuwari New Jhargram Purulia Modern Song Purulia Romantic Song.mp3 </v>
       </c>
       <c r="B35" t="str">
-        <v>https://puruliadj.in/download/649/purnimar_bhalobasha_singer_-_purnima_mandi_new_purulia_song</v>
+        <v>https://puruliadj.in/download/664/ami_kuwara_tui_kuwari_new_jhargram_purulia_modern_song_purulia_romantic_song</v>
       </c>
       <c r="C35" t="str">
-        <v>https://puruliadj.in/files/download/id/649</v>
+        <v>https://puruliadj.in/files/download/id/664</v>
       </c>
       <c r="D35" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E35" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F35" t="str">
-        <v>class</v>
+        <v>5.64 mb</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v xml:space="preserve">Mon Vitore Likhbo Re Tor Nam Singer - Purnima Mandi New Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Chamra Tolai Nachbo Dujon Bihar Dine Piu Rani Mahato New Purulia Jhargram New Song.mp3 </v>
       </c>
       <c r="B36" t="str">
-        <v>https://puruliadj.in/download/644/mon_vitore_likhbo_re_tor_nam_singer_-_purnima_mandi_new_jhumur_song</v>
+        <v>https://puruliadj.in/download/662/chamra_tolai_nachbo_dujon_bihar_dine_piu_rani_mahato_new_purulia_jhargram_new_song</v>
       </c>
       <c r="C36" t="str">
-        <v>https://puruliadj.in/files/download/id/644</v>
+        <v>https://puruliadj.in/files/download/id/662</v>
       </c>
       <c r="D36" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E36" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F36" t="str">
         <v>class</v>
@@ -1124,79 +1124,79 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v xml:space="preserve">Baba Maye Dibek Biha Purnima Mandi Mohan Baskey New Purulia Sad Song.mp3 </v>
+        <v xml:space="preserve">Cholka Cholka Pare Jacha Amar Kakher Kalshi Singer - AJ Lipini New Jhargram Purulia Song.mp3 </v>
       </c>
       <c r="B37" t="str">
-        <v>https://puruliadj.in/download/635/baba_maye_dibek_biha_purnima_mandi_mohan_baskey_new_purulia_sad_song</v>
+        <v>https://puruliadj.in/download/657/cholka_cholka_pare_jacha_amar_kakher_kalshi_singer_-_aj_lipini_new_jhargram_purulia_song</v>
       </c>
       <c r="C37" t="str">
-        <v>https://puruliadj.in/files/download/id/635</v>
+        <v>https://puruliadj.in/files/download/id/657</v>
       </c>
       <c r="D37" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E37" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F37" t="str">
-        <v>class</v>
+        <v>5.07 mb</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v xml:space="preserve">Young Bandhu Dharo Hat Singer - Purnima Mandi New Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Tor Bihar Pendal Ami Bonaichi Singer - Poritosh nd AJ Lipini  New Purulia Sed Jhargram Jhumur Song.mp3 </v>
       </c>
       <c r="B38" t="str">
-        <v>https://puruliadj.in/download/629/young_bandhu_dharo_hat_singer_-_purnima_mandi_new_jhumur_song</v>
+        <v>https://puruliadj.in/download/656/tor_bihar_pendal_ami_bonaichi_singer_-_poritosh_nd_aj_lipini__new_purulia_sed_jhargram_jhumur_song</v>
       </c>
       <c r="C38" t="str">
-        <v>https://puruliadj.in/files/download/id/629</v>
+        <v>https://puruliadj.in/files/download/id/656</v>
       </c>
       <c r="D38" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E38" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F38" t="str">
-        <v>9.19 mb</v>
+        <v>8.85 mb</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v xml:space="preserve">Bulu Sada School Dress - Holi Version Singer - Jagadish.mp3 </v>
+        <v xml:space="preserve">Lukai Lukai Kandis Na Valoi hobe tor bor Singer - Paritosh Mahata AJ Lipini.mp3 </v>
       </c>
       <c r="B39" t="str">
-        <v>https://puruliadj.in/download/594/bulu_sada_school_dress_-_holi_version_singer_-_jagadish</v>
+        <v>https://puruliadj.in/download/655/lukai_lukai_kandis_na_valoi_hobe_tor_bor_singer_-_paritosh_mahata_aj_lipini</v>
       </c>
       <c r="C39" t="str">
-        <v>https://puruliadj.in/files/download/id/594</v>
+        <v>https://puruliadj.in/files/download/id/655</v>
       </c>
       <c r="D39" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E39" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F39" t="str">
-        <v>6.2 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v xml:space="preserve">Mon Gelo Pichhla Shankar Tantubai Mira Das New Purulia Romantic Song.mp3 </v>
+        <v xml:space="preserve">Ghagra Bali Re Perit Hoye Jaba Singer - Kumar Paritosh Mahata New Jhargram Jhumur Song.mp3 </v>
       </c>
       <c r="B40" t="str">
-        <v>https://puruliadj.in/download/593/mon_gelo_pichhla_shankar_tantubai_mira_das_new_purulia_romantic_song</v>
+        <v>https://puruliadj.in/download/654/ghagra_bali_re_perit_hoye_jaba_singer_-_kumar_paritosh_mahata_new_jhargram_jhumur_song</v>
       </c>
       <c r="C40" t="str">
-        <v>https://puruliadj.in/files/download/id/593</v>
+        <v>https://puruliadj.in/files/download/id/654</v>
       </c>
       <c r="D40" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E40" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F40" t="str">
         <v>class</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v xml:space="preserve">Amar Sathiya New Purulia Sad Song Singer - Sanjeeb Kumar Rs Sailendra.mp3 </v>
+        <v xml:space="preserve">Ai Dekhe Ja Purulia Jhargram Bakura Singer - Purnima Mandi New Jhumur Song.mp3 </v>
       </c>
       <c r="B41" t="str">
-        <v>https://puruliadj.in/download/588/amar_sathiya_new_purulia_sad_song_singer_-_sanjeeb_kumar_rs_sailendra</v>
+        <v>https://puruliadj.in/download/652/ai_dekhe_ja_purulia_jhargram_bakura_singer_-_purnima_mandi_new_jhumur_song</v>
       </c>
       <c r="C41" t="str">
-        <v>https://puruliadj.in/files/download/id/588</v>
+        <v>https://puruliadj.in/files/download/id/652</v>
       </c>
       <c r="D41" t="str">
         <v>(New Purulia Songs)</v>
@@ -1219,18 +1219,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F41" t="str">
-        <v>7.82 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v xml:space="preserve">Ami O Iba Galai Dori Heart Touching Sad Song Rs Sailendra Bablu Sahis.mp3 </v>
+        <v xml:space="preserve">Young Bandhu Dharo Hat Singer - Purnima Mandi New Jhumur Song - Download.mp3 </v>
       </c>
       <c r="B42" t="str">
-        <v>https://puruliadj.in/download/587/ami_o_iba_galai_dori_heart_touching_sad_song_rs_sailendra_bablu_sahis</v>
+        <v>https://puruliadj.in/download/651/young_bandhu_dharo_hat_singer_-_purnima_mandi_new_jhumur_song_-_download</v>
       </c>
       <c r="C42" t="str">
-        <v>https://puruliadj.in/files/download/id/587</v>
+        <v>https://puruliadj.in/files/download/id/651</v>
       </c>
       <c r="D42" t="str">
         <v>(New Purulia Songs)</v>
@@ -1239,18 +1239,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F42" t="str">
-        <v>6.94 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v xml:space="preserve">Tor Bihar Din Chamra Agun Lagai Diba New Purulia Sad Song Kundan Kumar.mp3 </v>
+        <v xml:space="preserve">Purnimar Bhalobasha Singer - Purnima Mandi New Purulia Song.mp3 </v>
       </c>
       <c r="B43" t="str">
-        <v>https://puruliadj.in/download/586/tor_bihar_din_chamra_agun_lagai_diba_new_purulia_sad_song_kundan_kumar</v>
+        <v>https://puruliadj.in/download/649/purnimar_bhalobasha_singer_-_purnima_mandi_new_purulia_song</v>
       </c>
       <c r="C43" t="str">
-        <v>https://puruliadj.in/files/download/id/586</v>
+        <v>https://puruliadj.in/files/download/id/649</v>
       </c>
       <c r="D43" t="str">
         <v>(New Purulia Songs)</v>
@@ -1264,13 +1264,13 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v xml:space="preserve">Toke Shudhu Bhalobasi New Purulia Sad Song Tokei Sudhu chai Rajesh Sahis.mp3 </v>
+        <v xml:space="preserve">Mon Vitore Likhbo Re Tor Nam Singer - Purnima Mandi New Jhumur Song.mp3 </v>
       </c>
       <c r="B44" t="str">
-        <v>https://puruliadj.in/download/585/toke_shudhu_bhalobasi_new_purulia_sad_song_tokei_sudhu_chai_rajesh_sahis</v>
+        <v>https://puruliadj.in/download/644/mon_vitore_likhbo_re_tor_nam_singer_-_purnima_mandi_new_jhumur_song</v>
       </c>
       <c r="C44" t="str">
-        <v>https://puruliadj.in/files/download/id/585</v>
+        <v>https://puruliadj.in/files/download/id/644</v>
       </c>
       <c r="D44" t="str">
         <v>(New Purulia Songs)</v>
@@ -1279,18 +1279,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F44" t="str">
-        <v>5.67 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v xml:space="preserve">Kalyug er Draupadi Purulia Song Raju Sahis Romantic Song.mp3 </v>
+        <v xml:space="preserve">Baba Maye Dibek Biha Purnima Mandi Mohan Baskey New Purulia Sad Song.mp3 </v>
       </c>
       <c r="B45" t="str">
-        <v>https://puruliadj.in/download/584/kalyug_er_draupadi_purulia_song_raju_sahis_romantic_song</v>
+        <v>https://puruliadj.in/download/635/baba_maye_dibek_biha_purnima_mandi_mohan_baskey_new_purulia_sad_song</v>
       </c>
       <c r="C45" t="str">
-        <v>https://puruliadj.in/files/download/id/584</v>
+        <v>https://puruliadj.in/files/download/id/635</v>
       </c>
       <c r="D45" t="str">
         <v>(New Purulia Songs)</v>
@@ -1299,58 +1299,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F45" t="str">
-        <v>4.47 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v xml:space="preserve">Biha Habar Pare Jan Part- 2 Bhule Tui Gelis Re Kundan Kumar Bewafa Song.mp3 </v>
+        <v xml:space="preserve">Young Bandhu Dharo Hat Singer - Purnima Mandi New Jhumur Song.mp3 </v>
       </c>
       <c r="B46" t="str">
-        <v>https://puruliadj.in/download/583/biha_habar_pare_jan_part-_2_bhule_tui_gelis_re_kundan_kumar_bewafa_song</v>
+        <v>https://puruliadj.in/download/629/young_bandhu_dharo_hat_singer_-_purnima_mandi_new_jhumur_song</v>
       </c>
       <c r="C46" t="str">
-        <v>https://puruliadj.in/files/download/id/583</v>
+        <v>https://puruliadj.in/files/download/id/629</v>
       </c>
       <c r="D46" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E46" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F46" t="str">
-        <v>class</v>
+        <v>9.19 mb</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v xml:space="preserve">Paharer Rani Ami Paharer Rani Josna Mahato New Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Bulu Sada School Dress - Holi Version Singer - Jagadish.mp3 </v>
       </c>
       <c r="B47" t="str">
-        <v>https://puruliadj.in/download/582/paharer_rani_ami_paharer_rani_josna_mahato_new_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/594/bulu_sada_school_dress_-_holi_version_singer_-_jagadish</v>
       </c>
       <c r="C47" t="str">
-        <v>https://puruliadj.in/files/download/id/582</v>
+        <v>https://puruliadj.in/files/download/id/594</v>
       </c>
       <c r="D47" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E47" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F47" t="str">
-        <v>class</v>
+        <v>6.2 mb</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v xml:space="preserve">Sigareter Dhobo Dhoua Kumar Paritosh Mahata AJ Lipini New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Mon Gelo Pichhla Shankar Tantubai Mira Das New Purulia Romantic Song.mp3 </v>
       </c>
       <c r="B48" t="str">
-        <v>https://puruliadj.in/download/581/sigareter_dhobo_dhoua_kumar_paritosh_mahata_aj_lipini_new_purulia_song</v>
+        <v>https://puruliadj.in/download/593/mon_gelo_pichhla_shankar_tantubai_mira_das_new_purulia_romantic_song</v>
       </c>
       <c r="C48" t="str">
-        <v>https://puruliadj.in/files/download/id/581</v>
+        <v>https://puruliadj.in/files/download/id/593</v>
       </c>
       <c r="D48" t="str">
         <v>(New Purulia Songs)</v>
@@ -1359,18 +1359,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F48" t="str">
-        <v>6.04 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v xml:space="preserve">Rangabati New Purulia Song Konika Karmakar - Kundan Kumar.mp3 </v>
+        <v xml:space="preserve">Amar Sathiya New Purulia Sad Song Singer - Sanjeeb Kumar Rs Sailendra.mp3 </v>
       </c>
       <c r="B49" t="str">
-        <v>https://puruliadj.in/download/580/rangabati_new_purulia_song_konika_karmakar_-_kundan_kumar</v>
+        <v>https://puruliadj.in/download/588/amar_sathiya_new_purulia_sad_song_singer_-_sanjeeb_kumar_rs_sailendra</v>
       </c>
       <c r="C49" t="str">
-        <v>https://puruliadj.in/files/download/id/580</v>
+        <v>https://puruliadj.in/files/download/id/588</v>
       </c>
       <c r="D49" t="str">
         <v>(New Purulia Songs)</v>
@@ -1379,38 +1379,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F49" t="str">
-        <v>class</v>
+        <v>7.82 mb</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v xml:space="preserve">Gaibo Jhumur Dhomsa Madoler Tale Jhargram Jhumar Song Paritosh Mahata New Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Ami O Iba Galai Dori Heart Touching Sad Song Rs Sailendra Bablu Sahis.mp3 </v>
       </c>
       <c r="B50" t="str">
-        <v>https://puruliadj.in/download/548/gaibo_jhumur_dhomsa_madoler_tale_jhargram_jhumar_song_paritosh_mahata_new_jhumur_song</v>
+        <v>https://puruliadj.in/download/587/ami_o_iba_galai_dori_heart_touching_sad_song_rs_sailendra_bablu_sahis</v>
       </c>
       <c r="C50" t="str">
-        <v>https://puruliadj.in/files/download/id/548</v>
+        <v>https://puruliadj.in/files/download/id/587</v>
       </c>
       <c r="D50" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E50" t="str">
-        <v>New Kurmali Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F50" t="str">
-        <v>class</v>
+        <v>6.94 mb</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v xml:space="preserve">Kotha Jaye Sajali Basor New Purulia Video Song Download Singer - Kundan Kumar.mp3 </v>
+        <v xml:space="preserve">Tor Bihar Din Chamra Agun Lagai Diba New Purulia Sad Song Kundan Kumar.mp3 </v>
       </c>
       <c r="B51" t="str">
-        <v>https://puruliadj.in/download/542/kotha_jaye_sajali_basor_new_purulia_video_song_download_singer_-_kundan_kumar</v>
+        <v>https://puruliadj.in/download/586/tor_bihar_din_chamra_agun_lagai_diba_new_purulia_sad_song_kundan_kumar</v>
       </c>
       <c r="C51" t="str">
-        <v>https://puruliadj.in/files/download/id/542</v>
+        <v>https://puruliadj.in/files/download/id/586</v>
       </c>
       <c r="D51" t="str">
         <v>(New Purulia Songs)</v>
@@ -1424,13 +1424,13 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v xml:space="preserve">Chhamda Tole Ami Bosbo Na Sad Song Rs Sailendra Kundan Kumar Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Toke Shudhu Bhalobasi New Purulia Sad Song Tokei Sudhu chai Rajesh Sahis.mp3 </v>
       </c>
       <c r="B52" t="str">
-        <v>https://puruliadj.in/download/541/chhamda_tole_ami_bosbo_na_sad_song_rs_sailendra_kundan_kumar_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/585/toke_shudhu_bhalobasi_new_purulia_sad_song_tokei_sudhu_chai_rajesh_sahis</v>
       </c>
       <c r="C52" t="str">
-        <v>https://puruliadj.in/files/download/id/541</v>
+        <v>https://puruliadj.in/files/download/id/585</v>
       </c>
       <c r="D52" t="str">
         <v>(New Purulia Songs)</v>
@@ -1439,18 +1439,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F52" t="str">
-        <v>class</v>
+        <v>5.67 mb</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v xml:space="preserve">Tor Birohe Purulia Sad Song Kundan Kumar Kanika Karmakar New Purulia Song Download.mp3 </v>
+        <v xml:space="preserve">Kalyug er Draupadi Purulia Song Raju Sahis Romantic Song.mp3 </v>
       </c>
       <c r="B53" t="str">
-        <v>https://puruliadj.in/download/540/tor_birohe_purulia_sad_song_kundan_kumar_kanika_karmakar_new_purulia_song_download</v>
+        <v>https://puruliadj.in/download/584/kalyug_er_draupadi_purulia_song_raju_sahis_romantic_song</v>
       </c>
       <c r="C53" t="str">
-        <v>https://puruliadj.in/files/download/id/540</v>
+        <v>https://puruliadj.in/files/download/id/584</v>
       </c>
       <c r="D53" t="str">
         <v>(New Purulia Songs)</v>
@@ -1459,18 +1459,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F53" t="str">
-        <v>class</v>
+        <v>4.47 mb</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v xml:space="preserve">Jholo Molo (Holi Version) Purulia Song - Kundan Kumar Kanika Karmakar New Purulia Video Song 2024 Download.mp3 </v>
+        <v xml:space="preserve">Biha Habar Pare Jan Part- 2 Bhule Tui Gelis Re Kundan Kumar Bewafa Song.mp3 </v>
       </c>
       <c r="B54" t="str">
-        <v>https://puruliadj.in/download/539/jholo_molo_%28holi_version%29_purulia_song_-_kundan_kumar_kanika_karmakar_new_purulia_video_song_2024_download</v>
+        <v>https://puruliadj.in/download/583/biha_habar_pare_jan_part-_2_bhule_tui_gelis_re_kundan_kumar_bewafa_song</v>
       </c>
       <c r="C54" t="str">
-        <v>https://puruliadj.in/files/download/id/539</v>
+        <v>https://puruliadj.in/files/download/id/583</v>
       </c>
       <c r="D54" t="str">
         <v>(New Purulia Songs)</v>
@@ -1479,24 +1479,24 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F54" t="str">
-        <v>6.98 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v xml:space="preserve">Tor Birohe Purulia Sad Song 2024 Kundan Kumar Kanika Karmakar Download New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Paharer Rani Ami Paharer Rani Josna Mahato New Jhargram Jhumur Song.mp3 </v>
       </c>
       <c r="B55" t="str">
-        <v>https://puruliadj.in/download/527/tor_birohe_purulia_sad_song_2024_kundan_kumar_kanika_karmakar_download_new_purulia_song</v>
+        <v>https://puruliadj.in/download/582/paharer_rani_ami_paharer_rani_josna_mahato_new_jhargram_jhumur_song</v>
       </c>
       <c r="C55" t="str">
-        <v>https://puruliadj.in/files/download/id/527</v>
+        <v>https://puruliadj.in/files/download/id/582</v>
       </c>
       <c r="D55" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E55" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F55" t="str">
         <v>class</v>
@@ -1504,33 +1504,33 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v xml:space="preserve">Bohu Diner Pore Dekha Anjali Mahato Purulia Jhargram Romantic Song.mp3 </v>
+        <v xml:space="preserve">Sigareter Dhobo Dhoua Kumar Paritosh Mahata AJ Lipini New Purulia Song.mp3 </v>
       </c>
       <c r="B56" t="str">
-        <v>https://puruliadj.in/download/513/bohu_diner_pore_dekha_anjali_mahato_purulia_jhargram_romantic_song</v>
+        <v>https://puruliadj.in/download/581/sigareter_dhobo_dhoua_kumar_paritosh_mahata_aj_lipini_new_purulia_song</v>
       </c>
       <c r="C56" t="str">
-        <v>https://puruliadj.in/files/download/id/513</v>
+        <v>https://puruliadj.in/files/download/id/581</v>
       </c>
       <c r="D56" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E56" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F56" t="str">
-        <v>class</v>
+        <v>6.04 mb</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v xml:space="preserve">Tui Hamke Bhule Ja Again Kundan Kumar New Purulia Sad Song Download.mp3 </v>
+        <v xml:space="preserve">Rangabati New Purulia Song Konika Karmakar - Kundan Kumar.mp3 </v>
       </c>
       <c r="B57" t="str">
-        <v>https://puruliadj.in/download/512/tui_hamke_bhule_ja_again_kundan_kumar_new_purulia_sad_song_download</v>
+        <v>https://puruliadj.in/download/580/rangabati_new_purulia_song_konika_karmakar_-_kundan_kumar</v>
       </c>
       <c r="C57" t="str">
-        <v>https://puruliadj.in/files/download/id/512</v>
+        <v>https://puruliadj.in/files/download/id/580</v>
       </c>
       <c r="D57" t="str">
         <v>(New Purulia Songs)</v>
@@ -1544,19 +1544,19 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v xml:space="preserve">Bhalobase Chili Re New Purulia Song Singer Kundan Kumar Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Gaibo Jhumur Dhomsa Madoler Tale Jhargram Jhumar Song Paritosh Mahata New Jhumur Song.mp3 </v>
       </c>
       <c r="B58" t="str">
-        <v>https://puruliadj.in/download/510/bhalobase_chili_re_new_purulia_song_singer_kundan_kumar_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/548/gaibo_jhumur_dhomsa_madoler_tale_jhargram_jhumar_song_paritosh_mahata_new_jhumur_song</v>
       </c>
       <c r="C58" t="str">
-        <v>https://puruliadj.in/files/download/id/510</v>
+        <v>https://puruliadj.in/files/download/id/548</v>
       </c>
       <c r="D58" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E58" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Kurmali Jhumur Songs</v>
       </c>
       <c r="F58" t="str">
         <v>class</v>
@@ -1564,13 +1564,13 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v xml:space="preserve">LOJJABOTI Part - 3 Kundan Kumar Kanika Karmakar New Purulia Romantic Song 2024.mp3 </v>
+        <v xml:space="preserve">Kotha Jaye Sajali Basor New Purulia Video Song Download Singer - Kundan Kumar.mp3 </v>
       </c>
       <c r="B59" t="str">
-        <v>https://puruliadj.in/download/509/lojjaboti_part_-_3_kundan_kumar_kanika_karmakar_new_purulia_romantic_song_2024</v>
+        <v>https://puruliadj.in/download/542/kotha_jaye_sajali_basor_new_purulia_video_song_download_singer_-_kundan_kumar</v>
       </c>
       <c r="C59" t="str">
-        <v>https://puruliadj.in/files/download/id/509</v>
+        <v>https://puruliadj.in/files/download/id/542</v>
       </c>
       <c r="D59" t="str">
         <v>(New Purulia Songs)</v>
@@ -1584,19 +1584,19 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v xml:space="preserve">Didi Tor Ghor Ar Jabo Nai New Jhargram Jhumur Song Singer Josna Mahato.mp3 </v>
+        <v xml:space="preserve">Chhamda Tole Ami Bosbo Na Sad Song Rs Sailendra Kundan Kumar Kanika Karmakar.mp3 </v>
       </c>
       <c r="B60" t="str">
-        <v>https://puruliadj.in/download/442/didi_tor_ghor_ar_jabo_nai_new_jhargram_jhumur_song_singer_josna_mahato</v>
+        <v>https://puruliadj.in/download/541/chhamda_tole_ami_bosbo_na_sad_song_rs_sailendra_kundan_kumar_kanika_karmakar</v>
       </c>
       <c r="C60" t="str">
-        <v>https://puruliadj.in/files/download/id/442</v>
+        <v>https://puruliadj.in/files/download/id/541</v>
       </c>
       <c r="D60" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E60" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F60" t="str">
         <v>class</v>
@@ -1604,19 +1604,19 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v xml:space="preserve">Jhargram Mela Chal Munur Mai Paritosh Mahata And Pomi Mohanta New Jhargram Jhumar Song.mp3 </v>
+        <v xml:space="preserve">Tor Birohe Purulia Sad Song Kundan Kumar Kanika Karmakar New Purulia Song Download.mp3 </v>
       </c>
       <c r="B61" t="str">
-        <v>https://puruliadj.in/download/436/jhargram_mela_chal_munur_mai_paritosh_mahata_and_pomi_mohanta_new_jhargram_jhumar_song</v>
+        <v>https://puruliadj.in/download/540/tor_birohe_purulia_sad_song_kundan_kumar_kanika_karmakar_new_purulia_song_download</v>
       </c>
       <c r="C61" t="str">
-        <v>https://puruliadj.in/files/download/id/436</v>
+        <v>https://puruliadj.in/files/download/id/540</v>
       </c>
       <c r="D61" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E61" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F61" t="str">
         <v>class</v>
@@ -1624,33 +1624,33 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v xml:space="preserve">Ogo Ooo Fulmoni Tui Havi New Purulia Jhumar Song Singer Paritosh Mahata.mp3 </v>
+        <v xml:space="preserve">Jholo Molo (Holi Version) Purulia Song - Kundan Kumar Kanika Karmakar New Purulia Video Song 2024 Download.mp3 </v>
       </c>
       <c r="B62" t="str">
-        <v>https://puruliadj.in/download/430/ogo_ooo_fulmoni_tui_havi_new_purulia_jhumar_song_singer_paritosh_mahata</v>
+        <v>https://puruliadj.in/download/539/jholo_molo_%28holi_version%29_purulia_song_-_kundan_kumar_kanika_karmakar_new_purulia_video_song_2024_download</v>
       </c>
       <c r="C62" t="str">
-        <v>https://puruliadj.in/files/download/id/430</v>
+        <v>https://puruliadj.in/files/download/id/539</v>
       </c>
       <c r="D62" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E62" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F62" t="str">
-        <v>class</v>
+        <v>6.98 mb</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v xml:space="preserve">Chhamda Tole Ami Bosbo Na Sad Song Rs Sailendra Kundan Kumar Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Tor Birohe Purulia Sad Song 2024 Kundan Kumar Kanika Karmakar Download New Purulia Song.mp3 </v>
       </c>
       <c r="B63" t="str">
-        <v>https://puruliadj.in/download/426/chhamda_tole_ami_bosbo_na_sad_song_rs_sailendra_kundan_kumar_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/527/tor_birohe_purulia_sad_song_2024_kundan_kumar_kanika_karmakar_download_new_purulia_song</v>
       </c>
       <c r="C63" t="str">
-        <v>https://puruliadj.in/files/download/id/426</v>
+        <v>https://puruliadj.in/files/download/id/527</v>
       </c>
       <c r="D63" t="str">
         <v>(New Purulia Songs)</v>
@@ -1664,33 +1664,33 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v xml:space="preserve">Pagal Premik New Purulia Song Singer- Sadananda Bauri Mampi das.mp3 </v>
+        <v xml:space="preserve">Bohu Diner Pore Dekha Anjali Mahato Purulia Jhargram Romantic Song.mp3 </v>
       </c>
       <c r="B64" t="str">
-        <v>https://puruliadj.in/download/416/pagal_premik_new_purulia_song_singer-_sadananda_bauri_mampi_das</v>
+        <v>https://puruliadj.in/download/513/bohu_diner_pore_dekha_anjali_mahato_purulia_jhargram_romantic_song</v>
       </c>
       <c r="C64" t="str">
-        <v>https://puruliadj.in/files/download/id/416</v>
+        <v>https://puruliadj.in/files/download/id/513</v>
       </c>
       <c r="D64" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E64" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F64" t="str">
-        <v>7.4 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v xml:space="preserve">Camera Man Joldi Focus Karo Paritosh Mahata DSLR Babu Fokas Karo.mp3 </v>
+        <v xml:space="preserve">Tui Hamke Bhule Ja Again Kundan Kumar New Purulia Sad Song Download.mp3 </v>
       </c>
       <c r="B65" t="str">
-        <v>https://puruliadj.in/download/411/camera_man_joldi_focus_karo_paritosh_mahata_dslr_babu_fokas_karo</v>
+        <v>https://puruliadj.in/download/512/tui_hamke_bhule_ja_again_kundan_kumar_new_purulia_sad_song_download</v>
       </c>
       <c r="C65" t="str">
-        <v>https://puruliadj.in/files/download/id/411</v>
+        <v>https://puruliadj.in/files/download/id/512</v>
       </c>
       <c r="D65" t="str">
         <v>(New Purulia Songs)</v>
@@ -1699,38 +1699,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F65" t="str">
-        <v>6.34 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v xml:space="preserve">Age Humke De Babur Mai Purulia Jhumur Special Dj Song Mix By - Dj Tapas M T.mp3 </v>
+        <v xml:space="preserve">Bhalobase Chili Re New Purulia Song Singer Kundan Kumar Kanika Karmakar.mp3 </v>
       </c>
       <c r="B66" t="str">
-        <v>https://puruliadj.in/download/409/age_humke_de_babur_mai_purulia_jhumur_special_dj_song_mix_by_-_dj_tapas_m_t</v>
+        <v>https://puruliadj.in/download/510/bhalobase_chili_re_new_purulia_song_singer_kundan_kumar_kanika_karmakar</v>
       </c>
       <c r="C66" t="str">
-        <v>https://puruliadj.in/files/download/id/409</v>
+        <v>https://puruliadj.in/files/download/id/510</v>
       </c>
       <c r="D66" t="str">
-        <v>(All Types Of Dj Remix Song)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E66" t="str">
-        <v>Purulia Special Jhumur Dj Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F66" t="str">
-        <v>4.76 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v xml:space="preserve">Mohini - Kundan Kumar Kanika Karmakar New Purulia Song Download 2024.mp3 </v>
+        <v xml:space="preserve">LOJJABOTI Part - 3 Kundan Kumar Kanika Karmakar New Purulia Romantic Song 2024.mp3 </v>
       </c>
       <c r="B67" t="str">
-        <v>https://puruliadj.in/download/310/mohini_-_kundan_kumar_kanika_karmakar_new_purulia_song_download_2024</v>
+        <v>https://puruliadj.in/download/509/lojjaboti_part_-_3_kundan_kumar_kanika_karmakar_new_purulia_romantic_song_2024</v>
       </c>
       <c r="C67" t="str">
-        <v>https://puruliadj.in/files/download/id/310</v>
+        <v>https://puruliadj.in/files/download/id/509</v>
       </c>
       <c r="D67" t="str">
         <v>(New Purulia Songs)</v>
@@ -1744,19 +1744,19 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v xml:space="preserve">Karr Jonne Sajechis Dulhan Purulia Sad Song Singer Kundan Kumar Kanika karmakar Bewafa Sajani.mp3 </v>
+        <v xml:space="preserve">Didi Tor Ghor Ar Jabo Nai New Jhargram Jhumur Song Singer Josna Mahato.mp3 </v>
       </c>
       <c r="B68" t="str">
-        <v>https://puruliadj.in/download/307/karr_jonne_sajechis_dulhan_purulia_sad_song_singer_kundan_kumar_kanika_karmakar_bewafa_sajani</v>
+        <v>https://puruliadj.in/download/442/didi_tor_ghor_ar_jabo_nai_new_jhargram_jhumur_song_singer_josna_mahato</v>
       </c>
       <c r="C68" t="str">
-        <v>https://puruliadj.in/files/download/id/307</v>
+        <v>https://puruliadj.in/files/download/id/442</v>
       </c>
       <c r="D68" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E68" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F68" t="str">
         <v>class</v>
@@ -1764,19 +1764,19 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v xml:space="preserve">Pohil Barshai Shankar Tantubai New Song Purulia Romantic.mp3 </v>
+        <v xml:space="preserve">Jhargram Mela Chal Munur Mai Paritosh Mahata And Pomi Mohanta New Jhargram Jhumar Song.mp3 </v>
       </c>
       <c r="B69" t="str">
-        <v>https://puruliadj.in/download/269/pohil_barshai_shankar_tantubai_new_song_purulia_romantic</v>
+        <v>https://puruliadj.in/download/436/jhargram_mela_chal_munur_mai_paritosh_mahata_and_pomi_mohanta_new_jhargram_jhumar_song</v>
       </c>
       <c r="C69" t="str">
-        <v>https://puruliadj.in/files/download/id/269</v>
+        <v>https://puruliadj.in/files/download/id/436</v>
       </c>
       <c r="D69" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E69" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F69" t="str">
         <v>class</v>
@@ -1784,19 +1784,19 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v xml:space="preserve">Tor Pagla Re Kundan Kumar Kanika Karmakar Purulia New Song 2024.mp3 </v>
+        <v xml:space="preserve">Ogo Ooo Fulmoni Tui Havi New Purulia Jhumar Song Singer Paritosh Mahata.mp3 </v>
       </c>
       <c r="B70" t="str">
-        <v>https://puruliadj.in/download/268/tor_pagla_re_kundan_kumar_kanika_karmakar_purulia_new_song_2024</v>
+        <v>https://puruliadj.in/download/430/ogo_ooo_fulmoni_tui_havi_new_purulia_jhumar_song_singer_paritosh_mahata</v>
       </c>
       <c r="C70" t="str">
-        <v>https://puruliadj.in/files/download/id/268</v>
+        <v>https://puruliadj.in/files/download/id/430</v>
       </c>
       <c r="D70" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E70" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F70" t="str">
         <v>class</v>
@@ -1804,13 +1804,13 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v xml:space="preserve">A Amar Champa Rani Sankar Tantubai Mira Das Purulia New Video Song Download 2024.mp3 </v>
+        <v xml:space="preserve">Chhamda Tole Ami Bosbo Na Sad Song Rs Sailendra Kundan Kumar Kanika Karmakar.mp3 </v>
       </c>
       <c r="B71" t="str">
-        <v>https://puruliadj.in/download/267/a_amar_champa_rani_sankar_tantubai_mira_das_purulia_new_video_song_download_2024</v>
+        <v>https://puruliadj.in/download/426/chhamda_tole_ami_bosbo_na_sad_song_rs_sailendra_kundan_kumar_kanika_karmakar</v>
       </c>
       <c r="C71" t="str">
-        <v>https://puruliadj.in/files/download/id/267</v>
+        <v>https://puruliadj.in/files/download/id/426</v>
       </c>
       <c r="D71" t="str">
         <v>(New Purulia Songs)</v>
@@ -1824,73 +1824,73 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v xml:space="preserve">Tor Sange Pirit Kora Chai Chumki Rani Mahata New Purulia Jhargram Song Download.mp3 </v>
+        <v xml:space="preserve">Pagal Premik New Purulia Song Singer- Sadananda Bauri Mampi das.mp3 </v>
       </c>
       <c r="B72" t="str">
-        <v>https://puruliadj.in/download/266/tor_sange_pirit_kora_chai_chumki_rani_mahata_new_purulia_jhargram_song_download</v>
+        <v>https://puruliadj.in/download/416/pagal_premik_new_purulia_song_singer-_sadananda_bauri_mampi_das</v>
       </c>
       <c r="C72" t="str">
-        <v>https://puruliadj.in/files/download/id/266</v>
+        <v>https://puruliadj.in/files/download/id/416</v>
       </c>
       <c r="D72" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E72" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F72" t="str">
-        <v>class</v>
+        <v>7.4 mb</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v xml:space="preserve">Muchki Hanse Monta Amar Mojali Piu Rani Mahata New Purulia Jhargram Song.mp3 </v>
+        <v xml:space="preserve">Camera Man Joldi Focus Karo Paritosh Mahata DSLR Babu Fokas Karo.mp3 </v>
       </c>
       <c r="B73" t="str">
-        <v>https://puruliadj.in/download/265/muchki_hanse_monta_amar_mojali_piu_rani_mahata_new_purulia_jhargram_song</v>
+        <v>https://puruliadj.in/download/411/camera_man_joldi_focus_karo_paritosh_mahata_dslr_babu_fokas_karo</v>
       </c>
       <c r="C73" t="str">
-        <v>https://puruliadj.in/files/download/id/265</v>
+        <v>https://puruliadj.in/files/download/id/411</v>
       </c>
       <c r="D73" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E73" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F73" t="str">
-        <v>8.99 mb</v>
+        <v>6.34 mb</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v xml:space="preserve">Fulmoni Ei Fulmoni Tui Hevi Dekhachis Parayani Paritosh New Song.mp3 </v>
+        <v xml:space="preserve">Age Humke De Babur Mai Purulia Jhumur Special Dj Song Mix By - Dj Tapas M T.mp3 </v>
       </c>
       <c r="B74" t="str">
-        <v>https://puruliadj.in/download/264/fulmoni_ei_fulmoni_tui_hevi_dekhachis_parayani_paritosh_new_song</v>
+        <v>https://puruliadj.in/download/409/age_humke_de_babur_mai_purulia_jhumur_special_dj_song_mix_by_-_dj_tapas_m_t</v>
       </c>
       <c r="C74" t="str">
-        <v>https://puruliadj.in/files/download/id/264</v>
+        <v>https://puruliadj.in/files/download/id/409</v>
       </c>
       <c r="D74" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(All Types Of Dj Remix Song)</v>
       </c>
       <c r="E74" t="str">
-        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
+        <v>Purulia Special Jhumur Dj Songs</v>
       </c>
       <c r="F74" t="str">
-        <v>8.97 mb</v>
+        <v>4.76 mb</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v xml:space="preserve">Jaan Ja Niyachis Sab Ghurai De Romantic Bewafa New Purulia Song Download 2024.mp3 </v>
+        <v xml:space="preserve">Mohini - Kundan Kumar Kanika Karmakar New Purulia Song Download 2024.mp3 </v>
       </c>
       <c r="B75" t="str">
-        <v>https://puruliadj.in/download/257/jaan_ja_niyachis_sab_ghurai_de_romantic_bewafa_new_purulia_song_download_2024</v>
+        <v>https://puruliadj.in/download/310/mohini_-_kundan_kumar_kanika_karmakar_new_purulia_song_download_2024</v>
       </c>
       <c r="C75" t="str">
-        <v>https://puruliadj.in/files/download/id/257</v>
+        <v>https://puruliadj.in/files/download/id/310</v>
       </c>
       <c r="D75" t="str">
         <v>(New Purulia Songs)</v>
@@ -1899,38 +1899,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F75" t="str">
-        <v>10.73 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v xml:space="preserve">Beha Kore Le Sajani Paritosh mahata New jhumur Music Download.mp3 </v>
+        <v xml:space="preserve">Karr Jonne Sajechis Dulhan Purulia Sad Song Singer Kundan Kumar Kanika karmakar Bewafa Sajani.mp3 </v>
       </c>
       <c r="B76" t="str">
-        <v>https://puruliadj.in/download/254/beha_kore_le_sajani_paritosh_mahata_new_jhumur_music_download</v>
+        <v>https://puruliadj.in/download/307/karr_jonne_sajechis_dulhan_purulia_sad_song_singer_kundan_kumar_kanika_karmakar_bewafa_sajani</v>
       </c>
       <c r="C76" t="str">
-        <v>https://puruliadj.in/files/download/id/254</v>
+        <v>https://puruliadj.in/files/download/id/307</v>
       </c>
       <c r="D76" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E76" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F76" t="str">
-        <v>8.56 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v xml:space="preserve">Garib Cheila Ka Vule Gali Paritosh Mahata Purulia New Song 2024.mp3 </v>
+        <v xml:space="preserve">Pohil Barshai Shankar Tantubai New Song Purulia Romantic.mp3 </v>
       </c>
       <c r="B77" t="str">
-        <v>https://puruliadj.in/download/253/garib_cheila_ka_vule_gali_paritosh_mahata_purulia_new_song_2024</v>
+        <v>https://puruliadj.in/download/269/pohil_barshai_shankar_tantubai_new_song_purulia_romantic</v>
       </c>
       <c r="C77" t="str">
-        <v>https://puruliadj.in/files/download/id/253</v>
+        <v>https://puruliadj.in/files/download/id/269</v>
       </c>
       <c r="D77" t="str">
         <v>(New Purulia Songs)</v>
@@ -1939,18 +1939,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F77" t="str">
-        <v>8.61 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v xml:space="preserve">Valis Na Re Babu Upar Najar A Shikari Taniya New Purulia Romantic Song Download.mp3 </v>
+        <v xml:space="preserve">Tor Pagla Re Kundan Kumar Kanika Karmakar Purulia New Song 2024.mp3 </v>
       </c>
       <c r="B78" t="str">
-        <v>https://puruliadj.in/download/252/valis_na_re_babu_upar_najar_a_shikari_taniya_new_purulia_romantic_song_download</v>
+        <v>https://puruliadj.in/download/268/tor_pagla_re_kundan_kumar_kanika_karmakar_purulia_new_song_2024</v>
       </c>
       <c r="C78" t="str">
-        <v>https://puruliadj.in/files/download/id/252</v>
+        <v>https://puruliadj.in/files/download/id/268</v>
       </c>
       <c r="D78" t="str">
         <v>(New Purulia Songs)</v>
@@ -1959,138 +1959,138 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F78" t="str">
-        <v>8.96 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v xml:space="preserve">Behan Ta Chang Chainga Chai Gann Badal Paul Purulia Song Download.mp3 </v>
+        <v xml:space="preserve">A Amar Champa Rani Sankar Tantubai Mira Das Purulia New Video Song Download 2024.mp3 </v>
       </c>
       <c r="B79" t="str">
-        <v>https://puruliadj.in/download/248/behan_ta_chang_chainga_chai_gann_badal_paul_purulia_song_download</v>
+        <v>https://puruliadj.in/download/267/a_amar_champa_rani_sankar_tantubai_mira_das_purulia_new_video_song_download_2024</v>
       </c>
       <c r="C79" t="str">
-        <v>https://puruliadj.in/files/download/id/248</v>
+        <v>https://puruliadj.in/files/download/id/267</v>
       </c>
       <c r="D79" t="str">
         <v>(New Purulia Songs)</v>
       </c>
       <c r="E79" t="str">
-        <v>Old Purulia Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F79" t="str">
-        <v>8.45 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v xml:space="preserve">Tuku Baasna Bhalo Sajona Moner Moton Singer- Rj Rajani Jhargram.mp3 </v>
+        <v xml:space="preserve">Tor Sange Pirit Kora Chai Chumki Rani Mahata New Purulia Jhargram Song Download.mp3 </v>
       </c>
       <c r="B80" t="str">
-        <v>https://puruliadj.in/download/247/tuku_baasna_bhalo_sajona_moner_moton_singer-_rj_rajani_jhargram</v>
+        <v>https://puruliadj.in/download/266/tor_sange_pirit_kora_chai_chumki_rani_mahata_new_purulia_jhargram_song_download</v>
       </c>
       <c r="C80" t="str">
-        <v>https://puruliadj.in/files/download/id/247</v>
+        <v>https://puruliadj.in/files/download/id/266</v>
       </c>
       <c r="D80" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E80" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F80" t="str">
-        <v>10.23 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v xml:space="preserve">Tor Amar Valobasha Viral Hoye Gelo Singer - Manoj Das Mira Das Romantic Song.mp3 </v>
+        <v xml:space="preserve">Muchki Hanse Monta Amar Mojali Piu Rani Mahata New Purulia Jhargram Song.mp3 </v>
       </c>
       <c r="B81" t="str">
-        <v>https://puruliadj.in/download/246/tor_amar_valobasha_viral_hoye_gelo_singer_-_manoj_das_mira_das_romantic_song</v>
+        <v>https://puruliadj.in/download/265/muchki_hanse_monta_amar_mojali_piu_rani_mahata_new_purulia_jhargram_song</v>
       </c>
       <c r="C81" t="str">
-        <v>https://puruliadj.in/files/download/id/246</v>
+        <v>https://puruliadj.in/files/download/id/265</v>
       </c>
       <c r="D81" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E81" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F81" t="str">
-        <v>10.62 mb</v>
+        <v>8.99 mb</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v xml:space="preserve">Monta Niye Nilo Sajana Singer- Josna Mahato Jhargram Modern Jhumur Gann.mp3 </v>
+        <v xml:space="preserve">Fulmoni Ei Fulmoni Tui Hevi Dekhachis Parayani Paritosh New Song.mp3 </v>
       </c>
       <c r="B82" t="str">
-        <v>https://puruliadj.in/download/245/monta_niye_nilo_sajana_singer-_josna_mahato_jhargram_modern_jhumur_gann</v>
+        <v>https://puruliadj.in/download/264/fulmoni_ei_fulmoni_tui_hevi_dekhachis_parayani_paritosh_new_song</v>
       </c>
       <c r="C82" t="str">
-        <v>https://puruliadj.in/files/download/id/245</v>
+        <v>https://puruliadj.in/files/download/id/264</v>
       </c>
       <c r="D82" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E82" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Modern Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F82" t="str">
-        <v>7.87 mb</v>
+        <v>8.97 mb</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v xml:space="preserve">Amake Vitor Ghore Dhoreche Jorai Singer Josna Mahato Jhargram New Romantic Video Song.mp3 </v>
+        <v xml:space="preserve">Jaan Ja Niyachis Sab Ghurai De Romantic Bewafa New Purulia Song Download 2024.mp3 </v>
       </c>
       <c r="B83" t="str">
-        <v>https://puruliadj.in/download/244/amake_vitor_ghore_dhoreche_jorai_singer_josna_mahato_jhargram_new_romantic_video_song</v>
+        <v>https://puruliadj.in/download/257/jaan_ja_niyachis_sab_ghurai_de_romantic_bewafa_new_purulia_song_download_2024</v>
       </c>
       <c r="C83" t="str">
-        <v>https://puruliadj.in/files/download/id/244</v>
+        <v>https://puruliadj.in/files/download/id/257</v>
       </c>
       <c r="D83" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E83" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F83" t="str">
-        <v>8.64 mb</v>
+        <v>10.73 mb</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v xml:space="preserve">Aager Bhalobasa Singer - Karno Kumar Purulia Sad Song.mp3 </v>
+        <v xml:space="preserve">Beha Kore Le Sajani Paritosh mahata New jhumur Music Download.mp3 </v>
       </c>
       <c r="B84" t="str">
-        <v>https://puruliadj.in/download/243/aager_bhalobasa_singer_-_karno_kumar_purulia_sad_song</v>
+        <v>https://puruliadj.in/download/254/beha_kore_le_sajani_paritosh_mahata_new_jhumur_music_download</v>
       </c>
       <c r="C84" t="str">
-        <v>https://puruliadj.in/files/download/id/243</v>
+        <v>https://puruliadj.in/files/download/id/254</v>
       </c>
       <c r="D84" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E84" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F84" t="str">
-        <v>9.5 mb</v>
+        <v>8.56 mb</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v xml:space="preserve">Je Dike Takai Tor Chobi Dekhi Re New Purulia Romantic Song.mp3 </v>
+        <v xml:space="preserve">Garib Cheila Ka Vule Gali Paritosh Mahata Purulia New Song 2024.mp3 </v>
       </c>
       <c r="B85" t="str">
-        <v>https://puruliadj.in/download/242/je_dike_takai_tor_chobi_dekhi_re_new_purulia_romantic_song</v>
+        <v>https://puruliadj.in/download/253/garib_cheila_ka_vule_gali_paritosh_mahata_purulia_new_song_2024</v>
       </c>
       <c r="C85" t="str">
-        <v>https://puruliadj.in/files/download/id/242</v>
+        <v>https://puruliadj.in/files/download/id/253</v>
       </c>
       <c r="D85" t="str">
         <v>(New Purulia Songs)</v>
@@ -2099,18 +2099,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F85" t="str">
-        <v>13.39 mb</v>
+        <v>8.61 mb</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v xml:space="preserve">Barabajarer Chora Singer - Josna Mahato New Romantic Jhumar Video Song.mp3 </v>
+        <v xml:space="preserve">Valis Na Re Babu Upar Najar A Shikari Taniya New Purulia Romantic Song Download.mp3 </v>
       </c>
       <c r="B86" t="str">
-        <v>https://puruliadj.in/download/241/barabajarer_chora_singer_-_josna_mahato_new_romantic_jhumar_video_song</v>
+        <v>https://puruliadj.in/download/252/valis_na_re_babu_upar_najar_a_shikari_taniya_new_purulia_romantic_song_download</v>
       </c>
       <c r="C86" t="str">
-        <v>https://puruliadj.in/files/download/id/241</v>
+        <v>https://puruliadj.in/files/download/id/252</v>
       </c>
       <c r="D86" t="str">
         <v>(New Purulia Songs)</v>
@@ -2119,58 +2119,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F86" t="str">
-        <v>9.94 mb</v>
+        <v>8.96 mb</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v xml:space="preserve">Vukur Mai Chok Mare Che New Purulia Song Natun Romantic Video Song.mp3 </v>
+        <v xml:space="preserve">Behan Ta Chang Chainga Chai Gann Badal Paul Purulia Song Download.mp3 </v>
       </c>
       <c r="B87" t="str">
-        <v>https://puruliadj.in/download/240/vukur_mai_chok_mare_che_new_purulia_song_natun_romantic_video_song</v>
+        <v>https://puruliadj.in/download/248/behan_ta_chang_chainga_chai_gann_badal_paul_purulia_song_download</v>
       </c>
       <c r="C87" t="str">
-        <v>https://puruliadj.in/files/download/id/240</v>
+        <v>https://puruliadj.in/files/download/id/248</v>
       </c>
       <c r="D87" t="str">
         <v>(New Purulia Songs)</v>
       </c>
       <c r="E87" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Old Purulia Mp3 Songs</v>
       </c>
       <c r="F87" t="str">
-        <v>10.54 mb</v>
+        <v>8.45 mb</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v xml:space="preserve">Amar Bhalobasa Kene Tui Bujhli Nai Karna Kumar New Purulia Sad Song.mp3 </v>
+        <v xml:space="preserve">Tuku Baasna Bhalo Sajona Moner Moton Singer- Rj Rajani Jhargram.mp3 </v>
       </c>
       <c r="B88" t="str">
-        <v>https://puruliadj.in/download/239/amar_bhalobasa_kene_tui_bujhli_nai_karna_kumar_new_purulia_sad_song</v>
+        <v>https://puruliadj.in/download/247/tuku_baasna_bhalo_sajona_moner_moton_singer-_rj_rajani_jhargram</v>
       </c>
       <c r="C88" t="str">
-        <v>https://puruliadj.in/files/download/id/239</v>
+        <v>https://puruliadj.in/files/download/id/247</v>
       </c>
       <c r="D88" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E88" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F88" t="str">
-        <v>8.58 mb</v>
+        <v>10.23 mb</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v xml:space="preserve">Dil Diye Dil Bhalobasa Kore Lena Re Shankar Tantubai New Purulia Video Song Download.mp3 </v>
+        <v xml:space="preserve">Tor Amar Valobasha Viral Hoye Gelo Singer - Manoj Das Mira Das Romantic Song.mp3 </v>
       </c>
       <c r="B89" t="str">
-        <v>https://puruliadj.in/download/238/dil_diye_dil_bhalobasa_kore_lena_re_shankar_tantubai_new_purulia_video_song_download</v>
+        <v>https://puruliadj.in/download/246/tor_amar_valobasha_viral_hoye_gelo_singer_-_manoj_das_mira_das_romantic_song</v>
       </c>
       <c r="C89" t="str">
-        <v>https://puruliadj.in/files/download/id/238</v>
+        <v>https://puruliadj.in/files/download/id/246</v>
       </c>
       <c r="D89" t="str">
         <v>(New Purulia Songs)</v>
@@ -2179,58 +2179,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F89" t="str">
-        <v>class</v>
+        <v>10.62 mb</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v xml:space="preserve">Tui Hamke Bhule Ja Holi Special (Romantic Version) Kundan Kumar Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Monta Niye Nilo Sajana Singer- Josna Mahato Jhargram Modern Jhumur Gann.mp3 </v>
       </c>
       <c r="B90" t="str">
-        <v>https://puruliadj.in/download/237/tui_hamke_bhule_ja_holi_special_%28romantic_version%29_kundan_kumar_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/245/monta_niye_nilo_sajana_singer-_josna_mahato_jhargram_modern_jhumur_gann</v>
       </c>
       <c r="C90" t="str">
-        <v>https://puruliadj.in/files/download/id/237</v>
+        <v>https://puruliadj.in/files/download/id/245</v>
       </c>
       <c r="D90" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E90" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F90" t="str">
-        <v>class</v>
+        <v>7.87 mb</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v xml:space="preserve">Thik Kare Bol Takhan Le Dakli Tuku Karna Kumar Mira Das New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Amake Vitor Ghore Dhoreche Jorai Singer Josna Mahato Jhargram New Romantic Video Song.mp3 </v>
       </c>
       <c r="B91" t="str">
-        <v>https://puruliadj.in/download/236/thik_kare_bol_takhan_le_dakli_tuku_karna_kumar_mira_das_new_purulia_song</v>
+        <v>https://puruliadj.in/download/244/amake_vitor_ghore_dhoreche_jorai_singer_josna_mahato_jhargram_new_romantic_video_song</v>
       </c>
       <c r="C91" t="str">
-        <v>https://puruliadj.in/files/download/id/236</v>
+        <v>https://puruliadj.in/files/download/id/244</v>
       </c>
       <c r="D91" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E91" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F91" t="str">
-        <v>class</v>
+        <v>8.64 mb</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v xml:space="preserve">Sun Go Babur Mai Singer Raju Sahis Janani New Purulia Video Song Download.mp3 </v>
+        <v xml:space="preserve">Aager Bhalobasa Singer - Karno Kumar Purulia Sad Song.mp3 </v>
       </c>
       <c r="B92" t="str">
-        <v>https://puruliadj.in/download/235/sun_go_babur_mai_singer_raju_sahis_janani_new_purulia_video_song_download</v>
+        <v>https://puruliadj.in/download/243/aager_bhalobasa_singer_-_karno_kumar_purulia_sad_song</v>
       </c>
       <c r="C92" t="str">
-        <v>https://puruliadj.in/files/download/id/235</v>
+        <v>https://puruliadj.in/files/download/id/243</v>
       </c>
       <c r="D92" t="str">
         <v>(New Purulia Songs)</v>
@@ -2239,18 +2239,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F92" t="str">
-        <v>11.52 mb</v>
+        <v>9.5 mb</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v xml:space="preserve">i Hate You Baby Break Up Song Singer Raju Sahis Janani New Purulia Sad Song.mp3 </v>
+        <v xml:space="preserve">Je Dike Takai Tor Chobi Dekhi Re New Purulia Romantic Song.mp3 </v>
       </c>
       <c r="B93" t="str">
-        <v>https://puruliadj.in/download/234/i_hate_you_baby_break_up_song_singer_raju_sahis_janani_new_purulia_sad_song</v>
+        <v>https://puruliadj.in/download/242/je_dike_takai_tor_chobi_dekhi_re_new_purulia_romantic_song</v>
       </c>
       <c r="C93" t="str">
-        <v>https://puruliadj.in/files/download/id/234</v>
+        <v>https://puruliadj.in/files/download/id/242</v>
       </c>
       <c r="D93" t="str">
         <v>(New Purulia Songs)</v>
@@ -2259,58 +2259,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F93" t="str">
-        <v>14.2 mb</v>
+        <v>13.39 mb</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v xml:space="preserve">Dj Aaylo Dachak Dachak Kore (Humming Power Bass) Dj Sourav Exclusive.mp3 </v>
+        <v xml:space="preserve">Barabajarer Chora Singer - Josna Mahato New Romantic Jhumar Video Song.mp3 </v>
       </c>
       <c r="B94" t="str">
-        <v>https://puruliadj.in/download/228/dj_aaylo_dachak_dachak_kore_%28humming_power_bass%29_dj_sourav_exclusive</v>
+        <v>https://puruliadj.in/download/241/barabajarer_chora_singer_-_josna_mahato_new_romantic_jhumar_video_song</v>
       </c>
       <c r="C94" t="str">
-        <v>https://puruliadj.in/files/download/id/228</v>
+        <v>https://puruliadj.in/files/download/id/241</v>
       </c>
       <c r="D94" t="str">
-        <v>(All Types Of Dj Remix Song)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E94" t="str">
-        <v>Purulia Special Jhumur Dj Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F94" t="str">
-        <v>9.16 mb</v>
+        <v>9.94 mb</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v xml:space="preserve">Babuar Mai Moye Moye Shikari Taniya Saraswati Puja Hit Song DJ GourRock.mp3 </v>
+        <v xml:space="preserve">Vukur Mai Chok Mare Che New Purulia Song Natun Romantic Video Song.mp3 </v>
       </c>
       <c r="B95" t="str">
-        <v>https://puruliadj.in/download/204/babuar_mai_moye_moye_shikari_taniya_saraswati_puja_hit_song_dj_gourrock</v>
+        <v>https://puruliadj.in/download/240/vukur_mai_chok_mare_che_new_purulia_song_natun_romantic_video_song</v>
       </c>
       <c r="C95" t="str">
-        <v>https://puruliadj.in/files/download/id/204</v>
+        <v>https://puruliadj.in/files/download/id/240</v>
       </c>
       <c r="D95" t="str">
-        <v>(DJ Remix Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E95" t="str">
-        <v>Purulia Dj Remix Songs (DjGour Rock)</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F95" t="str">
-        <v>7.96 mb</v>
+        <v>10.54 mb</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v xml:space="preserve">Madhubala Re Shikari Taniya New Purulia Viral Trending Song Download.mp3 </v>
+        <v xml:space="preserve">Amar Bhalobasa Kene Tui Bujhli Nai Karna Kumar New Purulia Sad Song.mp3 </v>
       </c>
       <c r="B96" t="str">
-        <v>https://puruliadj.in/download/195/madhubala_re_shikari_taniya_new_purulia_viral_trending_song_download</v>
+        <v>https://puruliadj.in/download/239/amar_bhalobasa_kene_tui_bujhli_nai_karna_kumar_new_purulia_sad_song</v>
       </c>
       <c r="C96" t="str">
-        <v>https://puruliadj.in/files/download/id/195</v>
+        <v>https://puruliadj.in/files/download/id/239</v>
       </c>
       <c r="D96" t="str">
         <v>(New Purulia Songs)</v>
@@ -2319,18 +2319,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F96" t="str">
-        <v>6.33 mb</v>
+        <v>8.58 mb</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v xml:space="preserve">Puruliya Katoi Achha Sundar Shankar Tantubai And Kanika Karmakar Purulia Song Download 2024.mp3 </v>
+        <v xml:space="preserve">Dil Diye Dil Bhalobasa Kore Lena Re Shankar Tantubai New Purulia Video Song Download.mp3 </v>
       </c>
       <c r="B97" t="str">
-        <v>https://puruliadj.in/download/192/puruliya_katoi_achha_sundar_shankar_tantubai_and_kanika_karmakar_purulia_song_download_2024</v>
+        <v>https://puruliadj.in/download/238/dil_diye_dil_bhalobasa_kore_lena_re_shankar_tantubai_new_purulia_video_song_download</v>
       </c>
       <c r="C97" t="str">
-        <v>https://puruliadj.in/files/download/id/192</v>
+        <v>https://puruliadj.in/files/download/id/238</v>
       </c>
       <c r="D97" t="str">
         <v>(New Purulia Songs)</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v xml:space="preserve">Jholo Molo Sari Tor Jholo Molo Trending Viral Shankar Tantubai Mira Das New Purulia Video Song 2024.mp3 </v>
+        <v xml:space="preserve">Tui Hamke Bhule Ja Holi Special (Romantic Version) Kundan Kumar Kanika Karmakar.mp3 </v>
       </c>
       <c r="B98" t="str">
-        <v>https://puruliadj.in/download/191/jholo_molo_sari_tor_jholo_molo_trending_viral_shankar_tantubai_mira_das_new_purulia_video_song_2024</v>
+        <v>https://puruliadj.in/download/237/tui_hamke_bhule_ja_holi_special_%28romantic_version%29_kundan_kumar_kanika_karmakar</v>
       </c>
       <c r="C98" t="str">
-        <v>https://puruliadj.in/files/download/id/191</v>
+        <v>https://puruliadj.in/files/download/id/237</v>
       </c>
       <c r="D98" t="str">
         <v>(New Purulia Songs)</v>
@@ -2359,18 +2359,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F98" t="str">
-        <v>7.31 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v xml:space="preserve">Gouri Tor Gora Gale Til Kundan Kumar Purulia New Song 2024 Saraswati Pujo Special.mp3 </v>
+        <v xml:space="preserve">Thik Kare Bol Takhan Le Dakli Tuku Karna Kumar Mira Das New Purulia Song.mp3 </v>
       </c>
       <c r="B99" t="str">
-        <v>https://puruliadj.in/download/178/gouri_tor_gora_gale_til_kundan_kumar_purulia_new_song_2024_saraswati_pujo_special</v>
+        <v>https://puruliadj.in/download/236/thik_kare_bol_takhan_le_dakli_tuku_karna_kumar_mira_das_new_purulia_song</v>
       </c>
       <c r="C99" t="str">
-        <v>https://puruliadj.in/files/download/id/178</v>
+        <v>https://puruliadj.in/files/download/id/236</v>
       </c>
       <c r="D99" t="str">
         <v>(New Purulia Songs)</v>
@@ -2384,33 +2384,33 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v xml:space="preserve">Dil Mera Hoila Diwana Anjali Mahato O Pan Bala Babu New Jhargram Jhumur Gann Download.mp3 </v>
+        <v xml:space="preserve">Sun Go Babur Mai Singer Raju Sahis Janani New Purulia Video Song Download.mp3 </v>
       </c>
       <c r="B100" t="str">
-        <v>https://puruliadj.in/download/177/dil_mera_hoila_diwana_anjali_mahato_o_pan_bala_babu_new_jhargram_jhumur_gann_download</v>
+        <v>https://puruliadj.in/download/235/sun_go_babur_mai_singer_raju_sahis_janani_new_purulia_video_song_download</v>
       </c>
       <c r="C100" t="str">
-        <v>https://puruliadj.in/files/download/id/177</v>
+        <v>https://puruliadj.in/files/download/id/235</v>
       </c>
       <c r="D100" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E100" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F100" t="str">
-        <v>class</v>
+        <v>11.52 mb</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v xml:space="preserve">Tuku Dhoro No Chelata Shankar Tantubai New Purulia Video Song 2024.mp3 </v>
+        <v xml:space="preserve">i Hate You Baby Break Up Song Singer Raju Sahis Janani New Purulia Sad Song.mp3 </v>
       </c>
       <c r="B101" t="str">
-        <v>https://puruliadj.in/download/176/tuku_dhoro_no_chelata_shankar_tantubai_new_purulia_video_song_2024</v>
+        <v>https://puruliadj.in/download/234/i_hate_you_baby_break_up_song_singer_raju_sahis_janani_new_purulia_sad_song</v>
       </c>
       <c r="C101" t="str">
-        <v>https://puruliadj.in/files/download/id/176</v>
+        <v>https://puruliadj.in/files/download/id/234</v>
       </c>
       <c r="D101" t="str">
         <v>(New Purulia Songs)</v>
@@ -2419,58 +2419,58 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F101" t="str">
-        <v>class</v>
+        <v>14.2 mb</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v xml:space="preserve">Tuku Bhalobasar Abhash Diya Ja New Purulia Romentic Song Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Dj Aaylo Dachak Dachak Kore (Humming Power Bass) Dj Sourav Exclusive.mp3 </v>
       </c>
       <c r="B102" t="str">
-        <v>https://puruliadj.in/download/175/tuku_bhalobasar_abhash_diya_ja_new_purulia_romentic_song_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/228/dj_aaylo_dachak_dachak_kore_%28humming_power_bass%29_dj_sourav_exclusive</v>
       </c>
       <c r="C102" t="str">
-        <v>https://puruliadj.in/files/download/id/175</v>
+        <v>https://puruliadj.in/files/download/id/228</v>
       </c>
       <c r="D102" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Types Of Dj Remix Song)</v>
       </c>
       <c r="E102" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Purulia Special Jhumur Dj Songs</v>
       </c>
       <c r="F102" t="str">
-        <v>class</v>
+        <v>9.16 mb</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v xml:space="preserve">Jakhon Toka Call Kari Pai Waiting Bandhabi 2 New Purulia Video Song 2024 Sanjeeb Kumar.mp3 </v>
+        <v xml:space="preserve">Babuar Mai Moye Moye Shikari Taniya Saraswati Puja Hit Song DJ GourRock.mp3 </v>
       </c>
       <c r="B103" t="str">
-        <v>https://puruliadj.in/download/172/jakhon_toka_call_kari_pai_waiting_bandhabi_2_new_purulia_video_song_2024_sanjeeb_kumar</v>
+        <v>https://puruliadj.in/download/204/babuar_mai_moye_moye_shikari_taniya_saraswati_puja_hit_song_dj_gourrock</v>
       </c>
       <c r="C103" t="str">
-        <v>https://puruliadj.in/files/download/id/172</v>
+        <v>https://puruliadj.in/files/download/id/204</v>
       </c>
       <c r="D103" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(DJ Remix Songs)</v>
       </c>
       <c r="E103" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Purulia Dj Remix Songs (DjGour Rock)</v>
       </c>
       <c r="F103" t="str">
-        <v>8.57 mb</v>
+        <v>7.96 mb</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v xml:space="preserve">Jali Bairali Tui Bewafa Sona kundan Kumar New Purulia Sad Song.mp3 </v>
+        <v xml:space="preserve">Madhubala Re Shikari Taniya New Purulia Viral Trending Song Download.mp3 </v>
       </c>
       <c r="B104" t="str">
-        <v>https://puruliadj.in/download/164/jali_bairali_tui_bewafa_sona_kundan_kumar_new_purulia_sad_song</v>
+        <v>https://puruliadj.in/download/195/madhubala_re_shikari_taniya_new_purulia_viral_trending_song_download</v>
       </c>
       <c r="C104" t="str">
-        <v>https://puruliadj.in/files/download/id/164</v>
+        <v>https://puruliadj.in/files/download/id/195</v>
       </c>
       <c r="D104" t="str">
         <v>(New Purulia Songs)</v>
@@ -2479,18 +2479,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F104" t="str">
-        <v>class</v>
+        <v>6.33 mb</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v xml:space="preserve">Boudi Lover Purulia New Song 2024 Kundan Kumar And Kanika Karmakar.mp3 </v>
+        <v xml:space="preserve">Puruliya Katoi Achha Sundar Shankar Tantubai And Kanika Karmakar Purulia Song Download 2024.mp3 </v>
       </c>
       <c r="B105" t="str">
-        <v>https://puruliadj.in/download/161/boudi_lover_purulia_new_song_2024_kundan_kumar_and_kanika_karmakar</v>
+        <v>https://puruliadj.in/download/192/puruliya_katoi_achha_sundar_shankar_tantubai_and_kanika_karmakar_purulia_song_download_2024</v>
       </c>
       <c r="C105" t="str">
-        <v>https://puruliadj.in/files/download/id/161</v>
+        <v>https://puruliadj.in/files/download/id/192</v>
       </c>
       <c r="D105" t="str">
         <v>(New Purulia Songs)</v>
@@ -2504,13 +2504,13 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v xml:space="preserve">Sari Tor Jholo Molo Shankar Tantubai Mira Das New Purulia Mp3 Song 2024 Download.mp3 </v>
+        <v xml:space="preserve">Jholo Molo Sari Tor Jholo Molo Trending Viral Shankar Tantubai Mira Das New Purulia Video Song 2024.mp3 </v>
       </c>
       <c r="B106" t="str">
-        <v>https://puruliadj.in/download/158/sari_tor_jholo_molo_shankar_tantubai_mira_das_new_purulia_mp3_song_2024_download</v>
+        <v>https://puruliadj.in/download/191/jholo_molo_sari_tor_jholo_molo_trending_viral_shankar_tantubai_mira_das_new_purulia_video_song_2024</v>
       </c>
       <c r="C106" t="str">
-        <v>https://puruliadj.in/files/download/id/158</v>
+        <v>https://puruliadj.in/files/download/id/191</v>
       </c>
       <c r="D106" t="str">
         <v>(New Purulia Songs)</v>
@@ -2519,44 +2519,44 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F106" t="str">
-        <v>class</v>
+        <v>7.31 mb</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v xml:space="preserve">Purulia Jhumar Dj Cholke Geli Go Toke Bhale (Heavy Vibration Dnc Mix) Dj Tiku X Dj Subhajit Sn.mp3 </v>
+        <v xml:space="preserve">Gouri Tor Gora Gale Til Kundan Kumar Purulia New Song 2024 Saraswati Pujo Special.mp3 </v>
       </c>
       <c r="B107" t="str">
-        <v>https://puruliadj.in/download/156/purulia_jhumar_dj_cholke_geli_go_toke_bhale_%28heavy_vibration_dnc_mix%29_dj_tiku_x_dj_subhajit_sn</v>
+        <v>https://puruliadj.in/download/178/gouri_tor_gora_gale_til_kundan_kumar_purulia_new_song_2024_saraswati_pujo_special</v>
       </c>
       <c r="C107" t="str">
-        <v>https://puruliadj.in/files/download/id/156</v>
+        <v>https://puruliadj.in/files/download/id/178</v>
       </c>
       <c r="D107" t="str">
-        <v>(All Types Of Dj Remix Song)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E107" t="str">
-        <v>Purulia Special Jhumur Dj Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F107" t="str">
-        <v>6.04 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v xml:space="preserve">Mon Ta Hamar Bhange Dili Singer Kanika Karmakar New Purulia Sad Song 2024.mp3 </v>
+        <v xml:space="preserve">Dil Mera Hoila Diwana Anjali Mahato O Pan Bala Babu New Jhargram Jhumur Gann Download.mp3 </v>
       </c>
       <c r="B108" t="str">
-        <v>https://puruliadj.in/download/139/mon_ta_hamar_bhange_dili_singer_kanika_karmakar_new_purulia_sad_song_2024</v>
+        <v>https://puruliadj.in/download/177/dil_mera_hoila_diwana_anjali_mahato_o_pan_bala_babu_new_jhargram_jhumur_gann_download</v>
       </c>
       <c r="C108" t="str">
-        <v>https://puruliadj.in/files/download/id/139</v>
+        <v>https://puruliadj.in/files/download/id/177</v>
       </c>
       <c r="D108" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E108" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F108" t="str">
         <v>class</v>
@@ -2564,33 +2564,33 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v xml:space="preserve">Aaj Tor Gaye Holud (Hard Power Bass) Shikari Taniya New Sad Dj Song Dj GourRock.mp3 </v>
+        <v xml:space="preserve">Tuku Dhoro No Chelata Shankar Tantubai New Purulia Video Song 2024.mp3 </v>
       </c>
       <c r="B109" t="str">
-        <v>https://puruliadj.in/download/131/aaj_tor_gaye_holud_%28hard_power_bass%29_shikari_taniya_new_sad_dj_song_dj_gourrock</v>
+        <v>https://puruliadj.in/download/176/tuku_dhoro_no_chelata_shankar_tantubai_new_purulia_video_song_2024</v>
       </c>
       <c r="C109" t="str">
-        <v>https://puruliadj.in/files/download/id/131</v>
+        <v>https://puruliadj.in/files/download/id/176</v>
       </c>
       <c r="D109" t="str">
-        <v>(DJ Remix Songs)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E109" t="str">
-        <v>Purulia Dj Remix Songs (DjGour Rock)</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F109" t="str">
-        <v>9.16 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v xml:space="preserve">Aager Bhalobasa Singer - Karno Kumar Purulia Sad Song 2024.mp3 </v>
+        <v xml:space="preserve">Tuku Bhalobasar Abhash Diya Ja New Purulia Romentic Song Kanika Karmakar.mp3 </v>
       </c>
       <c r="B110" t="str">
-        <v>https://puruliadj.in/download/119/aager_bhalobasa_singer_-_karno_kumar_purulia_sad_song_2024</v>
+        <v>https://puruliadj.in/download/175/tuku_bhalobasar_abhash_diya_ja_new_purulia_romentic_song_kanika_karmakar</v>
       </c>
       <c r="C110" t="str">
-        <v>https://puruliadj.in/files/download/id/119</v>
+        <v>https://puruliadj.in/files/download/id/175</v>
       </c>
       <c r="D110" t="str">
         <v>(New Purulia Songs)</v>
@@ -2599,18 +2599,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F110" t="str">
-        <v>9.5 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v xml:space="preserve">Sukhe Thakis Swamir Ghare Shankar Tantubai Mira Das New Purulia Sad Song 2024.mp3 </v>
+        <v xml:space="preserve">Jakhon Toka Call Kari Pai Waiting Bandhabi 2 New Purulia Video Song 2024 Sanjeeb Kumar.mp3 </v>
       </c>
       <c r="B111" t="str">
-        <v>https://puruliadj.in/download/118/sukhe_thakis_swamir_ghare_shankar_tantubai_mira_das_new_purulia_sad_song_2024</v>
+        <v>https://puruliadj.in/download/172/jakhon_toka_call_kari_pai_waiting_bandhabi_2_new_purulia_video_song_2024_sanjeeb_kumar</v>
       </c>
       <c r="C111" t="str">
-        <v>https://puruliadj.in/files/download/id/118</v>
+        <v>https://puruliadj.in/files/download/id/172</v>
       </c>
       <c r="D111" t="str">
         <v>(New Purulia Songs)</v>
@@ -2619,18 +2619,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F111" t="str">
-        <v>15.96 mb</v>
+        <v>8.57 mb</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v xml:space="preserve">Tui Hamke Bhule Ja Re Pagla 2 Singer Kundan Kumar New Purulia Trending Song Download.mp3 </v>
+        <v xml:space="preserve">Jali Bairali Tui Bewafa Sona kundan Kumar New Purulia Sad Song.mp3 </v>
       </c>
       <c r="B112" t="str">
-        <v>https://puruliadj.in/download/116/tui_hamke_bhule_ja_re_pagla_2_singer_kundan_kumar_new_purulia_trending_song_download</v>
+        <v>https://puruliadj.in/download/164/jali_bairali_tui_bewafa_sona_kundan_kumar_new_purulia_sad_song</v>
       </c>
       <c r="C112" t="str">
-        <v>https://puruliadj.in/files/download/id/116</v>
+        <v>https://puruliadj.in/files/download/id/164</v>
       </c>
       <c r="D112" t="str">
         <v>(New Purulia Songs)</v>
@@ -2644,13 +2644,13 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v xml:space="preserve">Bewafa Sajani New Purulia Sad Song Kundan Kumar Kanika Karmakar Purulia Viral Song Download.mp3 </v>
+        <v xml:space="preserve">Boudi Lover Purulia New Song 2024 Kundan Kumar And Kanika Karmakar.mp3 </v>
       </c>
       <c r="B113" t="str">
-        <v>https://puruliadj.in/download/115/bewafa_sajani_new_purulia_sad_song_kundan_kumar_kanika_karmakar_purulia_viral_song_download</v>
+        <v>https://puruliadj.in/download/161/boudi_lover_purulia_new_song_2024_kundan_kumar_and_kanika_karmakar</v>
       </c>
       <c r="C113" t="str">
-        <v>https://puruliadj.in/files/download/id/115</v>
+        <v>https://puruliadj.in/files/download/id/161</v>
       </c>
       <c r="D113" t="str">
         <v>(New Purulia Songs)</v>
@@ -2659,18 +2659,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F113" t="str">
-        <v>15.42 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v xml:space="preserve">Ai Re Ai Re Barsha Tui Dhire Dhire Ai Shikari Taniya New Purulia Song Download.mp3 </v>
+        <v xml:space="preserve">Sari Tor Jholo Molo Shankar Tantubai Mira Das New Purulia Mp3 Song 2024 Download.mp3 </v>
       </c>
       <c r="B114" t="str">
-        <v>https://puruliadj.in/download/100/ai_re_ai_re_barsha_tui_dhire_dhire_ai_shikari_taniya_new_purulia_song_download</v>
+        <v>https://puruliadj.in/download/158/sari_tor_jholo_molo_shankar_tantubai_mira_das_new_purulia_mp3_song_2024_download</v>
       </c>
       <c r="C114" t="str">
-        <v>https://puruliadj.in/files/download/id/100</v>
+        <v>https://puruliadj.in/files/download/id/158</v>
       </c>
       <c r="D114" t="str">
         <v>(New Purulia Songs)</v>
@@ -2679,38 +2679,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F114" t="str">
-        <v>10.93 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v xml:space="preserve">Buka Ban Vange Dili Chokher Ishara Kanika Karmakar New Purulia Romantic Song Download.mp3 </v>
+        <v xml:space="preserve">Purulia Jhumar Dj Cholke Geli Go Toke Bhale (Heavy Vibration Dnc Mix) Dj Tiku X Dj Subhajit Sn.mp3 </v>
       </c>
       <c r="B115" t="str">
-        <v>https://puruliadj.in/download/99/buka_ban_vange_dili_chokher_ishara_kanika_karmakar_new_purulia_romantic_song_download</v>
+        <v>https://puruliadj.in/download/156/purulia_jhumar_dj_cholke_geli_go_toke_bhale_%28heavy_vibration_dnc_mix%29_dj_tiku_x_dj_subhajit_sn</v>
       </c>
       <c r="C115" t="str">
-        <v>https://puruliadj.in/files/download/id/99</v>
+        <v>https://puruliadj.in/files/download/id/156</v>
       </c>
       <c r="D115" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Types Of Dj Remix Song)</v>
       </c>
       <c r="E115" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Purulia Special Jhumur Dj Songs</v>
       </c>
       <c r="F115" t="str">
-        <v>class</v>
+        <v>6.04 mb</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v xml:space="preserve">Kotha Diye Chhili Saraswati Puja Special Kundan Kumar Kanika Karmakar Purulia New Song.mp3 </v>
+        <v xml:space="preserve">Mon Ta Hamar Bhange Dili Singer Kanika Karmakar New Purulia Sad Song 2024.mp3 </v>
       </c>
       <c r="B116" t="str">
-        <v>https://puruliadj.in/download/93/kotha_diye_chhili_saraswati_puja_special_kundan_kumar_kanika_karmakar_purulia_new_song</v>
+        <v>https://puruliadj.in/download/139/mon_ta_hamar_bhange_dili_singer_kanika_karmakar_new_purulia_sad_song_2024</v>
       </c>
       <c r="C116" t="str">
-        <v>https://puruliadj.in/files/download/id/93</v>
+        <v>https://puruliadj.in/files/download/id/139</v>
       </c>
       <c r="D116" t="str">
         <v>(New Purulia Songs)</v>
@@ -2724,33 +2724,33 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v xml:space="preserve">Bou Ta Jodi Bika Jaitho Bike (Jhumur Dance Mix) Dj Ritesh Cky.mp3.mp3 </v>
+        <v xml:space="preserve">Aaj Tor Gaye Holud (Hard Power Bass) Shikari Taniya New Sad Dj Song Dj GourRock.mp3 </v>
       </c>
       <c r="B117" t="str">
-        <v>https://puruliadj.in/download/81/bou_ta_jodi_bika_jaitho_bike_%28jhumur_dance_mix%29_dj_ritesh_cky</v>
+        <v>https://puruliadj.in/download/131/aaj_tor_gaye_holud_%28hard_power_bass%29_shikari_taniya_new_sad_dj_song_dj_gourrock</v>
       </c>
       <c r="C117" t="str">
-        <v>https://puruliadj.in/files/download/id/81</v>
+        <v>https://puruliadj.in/files/download/id/131</v>
       </c>
       <c r="D117" t="str">
-        <v>(All Types Of Dj Remix Song)</v>
+        <v>(DJ Remix Songs)</v>
       </c>
       <c r="E117" t="str">
-        <v>Purulia Special Jhumur Dj Songs</v>
+        <v>Purulia Dj Remix Songs (DjGour Rock)</v>
       </c>
       <c r="F117" t="str">
-        <v>12.33 mb</v>
+        <v>9.16 mb</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v xml:space="preserve">Mone Pore Go New Purulia Sad Song Mallik Mahato Jhumur.mp3 </v>
+        <v xml:space="preserve">Aager Bhalobasa Singer - Karno Kumar Purulia Sad Song 2024.mp3 </v>
       </c>
       <c r="B118" t="str">
-        <v>https://puruliadj.in/download/77/mone_pore_go_new_purulia_sad_song_mallik_mahato_jhumur</v>
+        <v>https://puruliadj.in/download/119/aager_bhalobasa_singer_-_karno_kumar_purulia_sad_song_2024</v>
       </c>
       <c r="C118" t="str">
-        <v>https://puruliadj.in/files/download/id/77</v>
+        <v>https://puruliadj.in/files/download/id/119</v>
       </c>
       <c r="D118" t="str">
         <v>(New Purulia Songs)</v>
@@ -2759,18 +2759,18 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F118" t="str">
-        <v>10.32 mb</v>
+        <v>9.5 mb</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v xml:space="preserve">Amar Rajkumai Re Neel Pori Re Jackson Shivani Singer Jagadish Priyanka New Purulia Song download.mp3 </v>
+        <v xml:space="preserve">Sukhe Thakis Swamir Ghare Shankar Tantubai Mira Das New Purulia Sad Song 2024.mp3 </v>
       </c>
       <c r="B119" t="str">
-        <v>https://puruliadj.in/download/75/amar_rajkumai_re_neel_pori_re_jackson_shivani_singer_jagadish_priyanka_new_purulia_song_download</v>
+        <v>https://puruliadj.in/download/118/sukhe_thakis_swamir_ghare_shankar_tantubai_mira_das_new_purulia_sad_song_2024</v>
       </c>
       <c r="C119" t="str">
-        <v>https://puruliadj.in/files/download/id/75</v>
+        <v>https://puruliadj.in/files/download/id/118</v>
       </c>
       <c r="D119" t="str">
         <v>(New Purulia Songs)</v>
@@ -2779,38 +2779,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F119" t="str">
-        <v>8.59 mb</v>
+        <v>15.96 mb</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v xml:space="preserve">Muchki Hanse Monta Amar Mojali Piu Rani Mahata New Purulia Jhargram Song Download.mp3 </v>
+        <v xml:space="preserve">Tui Hamke Bhule Ja Re Pagla 2 Singer Kundan Kumar New Purulia Trending Song Download.mp3 </v>
       </c>
       <c r="B120" t="str">
-        <v>https://puruliadj.in/download/74/muchki_hanse_monta_amar_mojali_piu_rani_mahata_new_purulia_jhargram_song_download</v>
+        <v>https://puruliadj.in/download/116/tui_hamke_bhule_ja_re_pagla_2_singer_kundan_kumar_new_purulia_trending_song_download</v>
       </c>
       <c r="C120" t="str">
-        <v>https://puruliadj.in/files/download/id/74</v>
+        <v>https://puruliadj.in/files/download/id/116</v>
       </c>
       <c r="D120" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E120" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F120" t="str">
-        <v>8.99 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v xml:space="preserve">Shampu Kara Chul Ure Ure Jai Mira Das New Purulia Song Download.mp3 </v>
+        <v xml:space="preserve">Bewafa Sajani New Purulia Sad Song Kundan Kumar Kanika Karmakar Purulia Viral Song Download.mp3 </v>
       </c>
       <c r="B121" t="str">
-        <v>https://puruliadj.in/download/71/shampu_kara_chul_ure_ure_jai_mira_das_new_purulia_song_download</v>
+        <v>https://puruliadj.in/download/115/bewafa_sajani_new_purulia_sad_song_kundan_kumar_kanika_karmakar_purulia_viral_song_download</v>
       </c>
       <c r="C121" t="str">
-        <v>https://puruliadj.in/files/download/id/71</v>
+        <v>https://puruliadj.in/files/download/id/115</v>
       </c>
       <c r="D121" t="str">
         <v>(New Purulia Songs)</v>
@@ -2819,44 +2819,44 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F121" t="str">
-        <v>class</v>
+        <v>15.42 mb</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v xml:space="preserve">Chithi Ta Pode Dekh Na Singer Khukumoni Mahata New Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Ai Re Ai Re Barsha Tui Dhire Dhire Ai Shikari Taniya New Purulia Song Download.mp3 </v>
       </c>
       <c r="B122" t="str">
-        <v>https://puruliadj.in/download/68/chithi_ta_pode_dekh_na_singer_khukumoni_mahata_new_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/100/ai_re_ai_re_barsha_tui_dhire_dhire_ai_shikari_taniya_new_purulia_song_download</v>
       </c>
       <c r="C122" t="str">
-        <v>https://puruliadj.in/files/download/id/68</v>
+        <v>https://puruliadj.in/files/download/id/100</v>
       </c>
       <c r="D122" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E122" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F122" t="str">
-        <v>class</v>
+        <v>10.93 mb</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v xml:space="preserve">Purulia Jhargram Ghurai Libo Toke Viral Song Paritosh Mahata Modern Jhargram Jhumur.mp3 </v>
+        <v xml:space="preserve">Buka Ban Vange Dili Chokher Ishara Kanika Karmakar New Purulia Romantic Song Download.mp3 </v>
       </c>
       <c r="B123" t="str">
-        <v>https://puruliadj.in/download/66/purulia_jhargram_ghurai_libo_toke_viral_song_paritosh_mahata_modern_jhargram_jhumur</v>
+        <v>https://puruliadj.in/download/99/buka_ban_vange_dili_chokher_ishara_kanika_karmakar_new_purulia_romantic_song_download</v>
       </c>
       <c r="C123" t="str">
-        <v>https://puruliadj.in/files/download/id/66</v>
+        <v>https://puruliadj.in/files/download/id/99</v>
       </c>
       <c r="D123" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E123" t="str">
-        <v>New Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F123" t="str">
         <v>class</v>
@@ -2864,13 +2864,13 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v xml:space="preserve">Amar Valobasha Kore Lena Re Shankar Tantubai New Purulia Song.mp3 </v>
+        <v xml:space="preserve">Kotha Diye Chhili Saraswati Puja Special Kundan Kumar Kanika Karmakar Purulia New Song.mp3 </v>
       </c>
       <c r="B124" t="str">
-        <v>https://puruliadj.in/download/62/amar_valobasha_kore_lena_re_shankar_tantubai_new_purulia_song</v>
+        <v>https://puruliadj.in/download/93/kotha_diye_chhili_saraswati_puja_special_kundan_kumar_kanika_karmakar_purulia_new_song</v>
       </c>
       <c r="C124" t="str">
-        <v>https://puruliadj.in/files/download/id/62</v>
+        <v>https://puruliadj.in/files/download/id/93</v>
       </c>
       <c r="D124" t="str">
         <v>(New Purulia Songs)</v>
@@ -2879,38 +2879,38 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F124" t="str">
-        <v>7.86 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v xml:space="preserve">Megha Rani Tuku Vija Le Shankar Tantubai Mira Das New Purulia MP3 Song.mp3 </v>
+        <v xml:space="preserve">Bou Ta Jodi Bika Jaitho Bike (Jhumur Dance Mix) Dj Ritesh Cky.mp3.mp3 </v>
       </c>
       <c r="B125" t="str">
-        <v>https://puruliadj.in/download/59/megha_rani_tuku_vija_le_shankar_tantubai_mira_das_new_purulia_mp3_song</v>
+        <v>https://puruliadj.in/download/81/bou_ta_jodi_bika_jaitho_bike_%28jhumur_dance_mix%29_dj_ritesh_cky</v>
       </c>
       <c r="C125" t="str">
-        <v>https://puruliadj.in/files/download/id/59</v>
+        <v>https://puruliadj.in/files/download/id/81</v>
       </c>
       <c r="D125" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Types Of Dj Remix Song)</v>
       </c>
       <c r="E125" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>Purulia Special Jhumur Dj Songs</v>
       </c>
       <c r="F125" t="str">
-        <v>10.97 mb</v>
+        <v>12.33 mb</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v xml:space="preserve">Tui Hamke Bhule Ja Re Pagla Kundan Kumar Kanika Karmakar New Purulia Viral Sad Song.mp3 </v>
+        <v xml:space="preserve">Mone Pore Go New Purulia Sad Song Mallik Mahato Jhumur.mp3 </v>
       </c>
       <c r="B126" t="str">
-        <v>https://puruliadj.in/download/58/tui_hamke_bhule_ja_re_pagla_kundan_kumar_kanika_karmakar_new_purulia_viral_sad_song</v>
+        <v>https://puruliadj.in/download/77/mone_pore_go_new_purulia_sad_song_mallik_mahato_jhumur</v>
       </c>
       <c r="C126" t="str">
-        <v>https://puruliadj.in/files/download/id/58</v>
+        <v>https://puruliadj.in/files/download/id/77</v>
       </c>
       <c r="D126" t="str">
         <v>(New Purulia Songs)</v>
@@ -2919,64 +2919,64 @@
         <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F126" t="str">
-        <v>class</v>
+        <v>10.32 mb</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v xml:space="preserve">Gaibo Jhumur Dhomsa Madoler Tale Jhargram Jhumar Song Paritosh Mahata.mp3 </v>
+        <v xml:space="preserve">Amar Rajkumai Re Neel Pori Re Jackson Shivani Singer Jagadish Priyanka New Purulia Song download.mp3 </v>
       </c>
       <c r="B127" t="str">
-        <v>https://puruliadj.in/download/19/gaibo_jhumur_dhomsa_madoler_tale_jhargram_jhumar_song_paritosh_mahata</v>
+        <v>https://puruliadj.in/download/75/amar_rajkumai_re_neel_pori_re_jackson_shivani_singer_jagadish_priyanka_new_purulia_song_download</v>
       </c>
       <c r="C127" t="str">
-        <v>https://puruliadj.in/files/download/id/19</v>
+        <v>https://puruliadj.in/files/download/id/75</v>
       </c>
       <c r="D127" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E127" t="str">
-        <v>Popular Jhumur Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F127" t="str">
-        <v>class</v>
+        <v>8.59 mb</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v xml:space="preserve">Toke Valo Basechi Go Pohil Darasone New Jhargram Viral Jhumar Song Paritosh Mahata.mp3 </v>
+        <v xml:space="preserve">Muchki Hanse Monta Amar Mojali Piu Rani Mahata New Purulia Jhargram Song Download.mp3 </v>
       </c>
       <c r="B128" t="str">
-        <v>https://puruliadj.in/download/17/toke_valo_basechi_go_pohil_darasone_new_jhargram_viral_jhumar_song_paritosh_mahata</v>
+        <v>https://puruliadj.in/download/74/muchki_hanse_monta_amar_mojali_piu_rani_mahata_new_purulia_jhargram_song_download</v>
       </c>
       <c r="C128" t="str">
-        <v>https://puruliadj.in/files/download/id/17</v>
+        <v>https://puruliadj.in/files/download/id/74</v>
       </c>
       <c r="D128" t="str">
-        <v>(All Festivals Songs)</v>
+        <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E128" t="str">
-        <v>New Kurmali Jhumur Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F128" t="str">
-        <v>class</v>
+        <v>8.99 mb</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v xml:space="preserve">Taha Reta Nana Tana Old Jhumur Song Singer - Anjali Mahato.mp3 </v>
+        <v xml:space="preserve">Shampu Kara Chul Ure Ure Jai Mira Das New Purulia Song Download.mp3 </v>
       </c>
       <c r="B129" t="str">
-        <v>https://puruliadj.in/download/14/taha_reta_nana_tana_old_jhumur_song_singer_-_anjali_mahato</v>
+        <v>https://puruliadj.in/download/71/shampu_kara_chul_ure_ure_jai_mira_das_new_purulia_song_download</v>
       </c>
       <c r="C129" t="str">
-        <v>https://puruliadj.in/files/download/id/14</v>
+        <v>https://puruliadj.in/files/download/id/71</v>
       </c>
       <c r="D129" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E129" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F129" t="str">
         <v>class</v>
@@ -2984,19 +2984,19 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v xml:space="preserve">Phool Pori Tui Michha Michhi Rag Koris Kene old Super Hit Jhumur Singer - Ajit Mahato.mp3 </v>
+        <v xml:space="preserve">Chithi Ta Pode Dekh Na Singer Khukumoni Mahata New Jhargram Jhumur Song.mp3 </v>
       </c>
       <c r="B130" t="str">
-        <v>https://puruliadj.in/download/13/phool_pori_tui_michha_michhi_rag_koris_kene_old_super_hit_jhumur_singer_-_ajit_mahato</v>
+        <v>https://puruliadj.in/download/68/chithi_ta_pode_dekh_na_singer_khukumoni_mahata_new_jhargram_jhumur_song</v>
       </c>
       <c r="C130" t="str">
-        <v>https://puruliadj.in/files/download/id/13</v>
+        <v>https://puruliadj.in/files/download/id/68</v>
       </c>
       <c r="D130" t="str">
         <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E130" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F130" t="str">
         <v>class</v>
@@ -3004,19 +3004,19 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v xml:space="preserve">Chal Sakhi Chal Palai Jabo Phooler Bagane Jhumur Song Ajit Mahata.mp3 </v>
+        <v xml:space="preserve">Purulia Jhargram Ghurai Libo Toke Viral Song Paritosh Mahata Modern Jhargram Jhumur.mp3 </v>
       </c>
       <c r="B131" t="str">
-        <v>https://puruliadj.in/download/12/chal_sakhi_chal_palai_jabo_phooler_bagane_jhumur_song_ajit_mahata</v>
+        <v>https://puruliadj.in/download/66/purulia_jhargram_ghurai_libo_toke_viral_song_paritosh_mahata_modern_jhargram_jhumur</v>
       </c>
       <c r="C131" t="str">
-        <v>https://puruliadj.in/files/download/id/12</v>
+        <v>https://puruliadj.in/files/download/id/66</v>
       </c>
       <c r="D131" t="str">
         <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E131" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F131" t="str">
         <v>class</v>
@@ -3024,59 +3024,59 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v xml:space="preserve">Kolikatar Konak Lota Malabatir Mala Gatha Singer - Bijoy Mahata.mp3 </v>
+        <v xml:space="preserve">Amar Valobasha Kore Lena Re Shankar Tantubai New Purulia Song.mp3 </v>
       </c>
       <c r="B132" t="str">
-        <v>https://puruliadj.in/download/11/kolikatar_konak_lota_malabatir_mala_gatha_singer_-_bijoy_mahata</v>
+        <v>https://puruliadj.in/download/62/amar_valobasha_kore_lena_re_shankar_tantubai_new_purulia_song</v>
       </c>
       <c r="C132" t="str">
-        <v>https://puruliadj.in/files/download/id/11</v>
+        <v>https://puruliadj.in/files/download/id/62</v>
       </c>
       <c r="D132" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E132" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F132" t="str">
-        <v>class</v>
+        <v>7.86 mb</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v xml:space="preserve">Kagoje Na Likho Bondhu Gachhe Likho Jhumur Song Ajit Mahato.mp3 </v>
+        <v xml:space="preserve">Megha Rani Tuku Vija Le Shankar Tantubai Mira Das New Purulia MP3 Song.mp3 </v>
       </c>
       <c r="B133" t="str">
-        <v>https://puruliadj.in/download/10/kagoje_na_likho_bondhu_gachhe_likho_jhumur_song_ajit_mahato</v>
+        <v>https://puruliadj.in/download/59/megha_rani_tuku_vija_le_shankar_tantubai_mira_das_new_purulia_mp3_song</v>
       </c>
       <c r="C133" t="str">
-        <v>https://puruliadj.in/files/download/id/10</v>
+        <v>https://puruliadj.in/files/download/id/59</v>
       </c>
       <c r="D133" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E133" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F133" t="str">
-        <v>class</v>
+        <v>10.97 mb</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v xml:space="preserve">Magh Fagun Chot Mase Jhumur Song Ajit Mahato.mp3 </v>
+        <v xml:space="preserve">Tui Hamke Bhule Ja Re Pagla Kundan Kumar Kanika Karmakar New Purulia Viral Sad Song.mp3 </v>
       </c>
       <c r="B134" t="str">
-        <v>https://puruliadj.in/download/9/magh_fagun_chot_mase_jhumur_song_ajit_mahato</v>
+        <v>https://puruliadj.in/download/58/tui_hamke_bhule_ja_re_pagla_kundan_kumar_kanika_karmakar_new_purulia_viral_sad_song</v>
       </c>
       <c r="C134" t="str">
-        <v>https://puruliadj.in/files/download/id/9</v>
+        <v>https://puruliadj.in/files/download/id/58</v>
       </c>
       <c r="D134" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(New Purulia Songs)</v>
       </c>
       <c r="E134" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Purulia Mp3 Songs</v>
       </c>
       <c r="F134" t="str">
         <v>class</v>
@@ -3084,19 +3084,19 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v xml:space="preserve">Sanjher Bela Jhore Jole Jate Chhili old Super Hit Jhumur Song Ajit Mahato.mp3 </v>
+        <v xml:space="preserve">Gaibo Jhumur Dhomsa Madoler Tale Jhargram Jhumar Song Paritosh Mahata.mp3 </v>
       </c>
       <c r="B135" t="str">
-        <v>https://puruliadj.in/download/8/sanjher_bela_jhore_jole_jate_chhili_old_super_hit_jhumur_song_ajit_mahato</v>
+        <v>https://puruliadj.in/download/19/gaibo_jhumur_dhomsa_madoler_tale_jhargram_jhumar_song_paritosh_mahata</v>
       </c>
       <c r="C135" t="str">
-        <v>https://puruliadj.in/files/download/id/8</v>
+        <v>https://puruliadj.in/files/download/id/19</v>
       </c>
       <c r="D135" t="str">
         <v>(New Jhargram Jhumur)</v>
       </c>
       <c r="E135" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>Popular Jhumur Songs</v>
       </c>
       <c r="F135" t="str">
         <v>class</v>
@@ -3104,19 +3104,19 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v xml:space="preserve">Jhumur Song Das Bachar Pore Dekha Howrah Station a Singer - Ajit Mahata.mp3 </v>
+        <v xml:space="preserve">Aadhadine Bhange Dili Piriter Phuta Phul Paritosh Mahato Sad Song.mp3 </v>
       </c>
       <c r="B136" t="str">
-        <v>https://puruliadj.in/download/7/jhumur_song_das_bachar_pore_dekha_howrah_station_a_singer_-_ajit_mahata</v>
+        <v>https://puruliadj.in/download/18/aadhadine_bhange_dili_piriter_phuta_phul_paritosh_mahato_sad_song</v>
       </c>
       <c r="C136" t="str">
-        <v>https://puruliadj.in/files/download/id/7</v>
+        <v>https://puruliadj.in/files/download/id/18</v>
       </c>
       <c r="D136" t="str">
-        <v>(New Jhargram Jhumur)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E136" t="str">
-        <v>Old Jhargram Jhumur Mp3 Songs</v>
+        <v>New Kurmali Jhumur Songs</v>
       </c>
       <c r="F136" t="str">
         <v>class</v>
@@ -3124,19 +3124,19 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v xml:space="preserve">Lojjaboti Ruper Raj Kumari Kundan Kumar Kanika Karmakar New Purulia Romantic Song.mp3 </v>
+        <v xml:space="preserve">Toke Valo Basechi Go Pohil Darasone New Jhargram Viral Jhumar Song Paritosh Mahata.mp3 </v>
       </c>
       <c r="B137" t="str">
-        <v>https://puruliadj.in/download/6/lojjaboti_ruper_raj_kumari_kundan_kumar_kanika_karmakar_new_purulia_romantic_song</v>
+        <v>https://puruliadj.in/download/17/toke_valo_basechi_go_pohil_darasone_new_jhargram_viral_jhumar_song_paritosh_mahata</v>
       </c>
       <c r="C137" t="str">
-        <v>https://puruliadj.in/files/download/id/6</v>
+        <v>https://puruliadj.in/files/download/id/17</v>
       </c>
       <c r="D137" t="str">
-        <v>(New Purulia Songs)</v>
+        <v>(All Festivals Songs)</v>
       </c>
       <c r="E137" t="str">
-        <v>New Purulia Mp3 Songs</v>
+        <v>New Kurmali Jhumur Songs</v>
       </c>
       <c r="F137" t="str">
         <v>class</v>
@@ -3144,13 +3144,13 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v xml:space="preserve">Tui Hamar Sagar Tui Hamar Nagar Old Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Taha Reta Nana Tana Old Jhumur Song Singer - Anjali Mahato.mp3 </v>
       </c>
       <c r="B138" t="str">
-        <v>https://puruliadj.in/download/5/tui_hamar_sagar_tui_hamar_nagar_old_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/14/taha_reta_nana_tana_old_jhumur_song_singer_-_anjali_mahato</v>
       </c>
       <c r="C138" t="str">
-        <v>https://puruliadj.in/files/download/id/5</v>
+        <v>https://puruliadj.in/files/download/id/14</v>
       </c>
       <c r="D138" t="str">
         <v>(New Jhargram Jhumur)</v>
@@ -3159,18 +3159,18 @@
         <v>Old Jhargram Jhumur Mp3 Songs</v>
       </c>
       <c r="F138" t="str">
-        <v>9.92 mb</v>
+        <v>class</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v xml:space="preserve">Sajani Go Valobasai Sakhi Gacher Full Tapas Mahata Old Jhumur Songs.mp3 </v>
+        <v xml:space="preserve">Phool Pori Tui Michha Michhi Rag Koris Kene old Super Hit Jhumur Singer - Ajit Mahato.mp3 </v>
       </c>
       <c r="B139" t="str">
-        <v>https://puruliadj.in/download/4/sajani_go_valobasai_sakhi_gacher_full_tapas_mahata_old_jhumur_songs</v>
+        <v>https://puruliadj.in/download/13/phool_pori_tui_michha_michhi_rag_koris_kene_old_super_hit_jhumur_singer_-_ajit_mahato</v>
       </c>
       <c r="C139" t="str">
-        <v>https://puruliadj.in/files/download/id/4</v>
+        <v>https://puruliadj.in/files/download/id/13</v>
       </c>
       <c r="D139" t="str">
         <v>(New Jhargram Jhumur)</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v xml:space="preserve">Fagun Ale Lage Baro Dar Paritosh Mahata Old Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Chal Sakhi Chal Palai Jabo Phooler Bagane Jhumur Song Ajit Mahata.mp3 </v>
       </c>
       <c r="B140" t="str">
-        <v>https://puruliadj.in/download/3/fagun_ale_lage_baro_dar_paritosh_mahata_old_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/12/chal_sakhi_chal_palai_jabo_phooler_bagane_jhumur_song_ajit_mahata</v>
       </c>
       <c r="C140" t="str">
-        <v>https://puruliadj.in/files/download/id/3</v>
+        <v>https://puruliadj.in/files/download/id/12</v>
       </c>
       <c r="D140" t="str">
         <v>(New Jhargram Jhumur)</v>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v xml:space="preserve">Sathi Aay Re Chumki Rani Mahata New Purulia Jhargram Jhumur Song.mp3 </v>
+        <v xml:space="preserve">Kolikatar Konak Lota Malabatir Mala Gatha Singer - Bijoy Mahata.mp3 </v>
       </c>
       <c r="B141" t="str">
-        <v>https://puruliadj.in/download/2/sathi_aay_re_chumki_rani_mahata_new_purulia_jhargram_jhumur_song</v>
+        <v>https://puruliadj.in/download/11/kolikatar_konak_lota_malabatir_mala_gatha_singer_-_bijoy_mahata</v>
       </c>
       <c r="C141" t="str">
-        <v>https://puruliadj.in/files/download/id/2</v>
+        <v>https://puruliadj.in/files/download/id/11</v>
       </c>
       <c r="D141" t="str">
         <v>(New Jhargram Jhumur)</v>
@@ -3224,27 +3224,207 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
+        <v xml:space="preserve">Kagoje Na Likho Bondhu Gachhe Likho Jhumur Song Ajit Mahato.mp3 </v>
+      </c>
+      <c r="B142" t="str">
+        <v>https://puruliadj.in/download/10/kagoje_na_likho_bondhu_gachhe_likho_jhumur_song_ajit_mahato</v>
+      </c>
+      <c r="C142" t="str">
+        <v>https://puruliadj.in/files/download/id/10</v>
+      </c>
+      <c r="D142" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E142" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F142" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v xml:space="preserve">Magh Fagun Chot Mase Jhumur Song Ajit Mahato.mp3 </v>
+      </c>
+      <c r="B143" t="str">
+        <v>https://puruliadj.in/download/9/magh_fagun_chot_mase_jhumur_song_ajit_mahato</v>
+      </c>
+      <c r="C143" t="str">
+        <v>https://puruliadj.in/files/download/id/9</v>
+      </c>
+      <c r="D143" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E143" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F143" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v xml:space="preserve">Sanjher Bela Jhore Jole Jate Chhili old Super Hit Jhumur Song Ajit Mahato.mp3 </v>
+      </c>
+      <c r="B144" t="str">
+        <v>https://puruliadj.in/download/8/sanjher_bela_jhore_jole_jate_chhili_old_super_hit_jhumur_song_ajit_mahato</v>
+      </c>
+      <c r="C144" t="str">
+        <v>https://puruliadj.in/files/download/id/8</v>
+      </c>
+      <c r="D144" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E144" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F144" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v xml:space="preserve">Jhumur Song Das Bachar Pore Dekha Howrah Station a Singer - Ajit Mahata.mp3 </v>
+      </c>
+      <c r="B145" t="str">
+        <v>https://puruliadj.in/download/7/jhumur_song_das_bachar_pore_dekha_howrah_station_a_singer_-_ajit_mahata</v>
+      </c>
+      <c r="C145" t="str">
+        <v>https://puruliadj.in/files/download/id/7</v>
+      </c>
+      <c r="D145" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E145" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F145" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v xml:space="preserve">Lojjaboti Ruper Raj Kumari Kundan Kumar Kanika Karmakar New Purulia Romantic Song.mp3 </v>
+      </c>
+      <c r="B146" t="str">
+        <v>https://puruliadj.in/download/6/lojjaboti_ruper_raj_kumari_kundan_kumar_kanika_karmakar_new_purulia_romantic_song</v>
+      </c>
+      <c r="C146" t="str">
+        <v>https://puruliadj.in/files/download/id/6</v>
+      </c>
+      <c r="D146" t="str">
+        <v>(New Purulia Songs)</v>
+      </c>
+      <c r="E146" t="str">
+        <v>New Purulia Mp3 Songs</v>
+      </c>
+      <c r="F146" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v xml:space="preserve">Tui Hamar Sagar Tui Hamar Nagar Old Jhargram Jhumur Song.mp3 </v>
+      </c>
+      <c r="B147" t="str">
+        <v>https://puruliadj.in/download/5/tui_hamar_sagar_tui_hamar_nagar_old_jhargram_jhumur_song</v>
+      </c>
+      <c r="C147" t="str">
+        <v>https://puruliadj.in/files/download/id/5</v>
+      </c>
+      <c r="D147" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E147" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F147" t="str">
+        <v>9.92 mb</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v xml:space="preserve">Sajani Go Valobasai Sakhi Gacher Full Tapas Mahata Old Jhumur Songs.mp3 </v>
+      </c>
+      <c r="B148" t="str">
+        <v>https://puruliadj.in/download/4/sajani_go_valobasai_sakhi_gacher_full_tapas_mahata_old_jhumur_songs</v>
+      </c>
+      <c r="C148" t="str">
+        <v>https://puruliadj.in/files/download/id/4</v>
+      </c>
+      <c r="D148" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E148" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F148" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v xml:space="preserve">Fagun Ale Lage Baro Dar Paritosh Mahata Old Jhargram Jhumur Song.mp3 </v>
+      </c>
+      <c r="B149" t="str">
+        <v>https://puruliadj.in/download/3/fagun_ale_lage_baro_dar_paritosh_mahata_old_jhargram_jhumur_song</v>
+      </c>
+      <c r="C149" t="str">
+        <v>https://puruliadj.in/files/download/id/3</v>
+      </c>
+      <c r="D149" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E149" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F149" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v xml:space="preserve">Sathi Aay Re Chumki Rani Mahata New Purulia Jhargram Jhumur Song.mp3 </v>
+      </c>
+      <c r="B150" t="str">
+        <v>https://puruliadj.in/download/2/sathi_aay_re_chumki_rani_mahata_new_purulia_jhargram_jhumur_song</v>
+      </c>
+      <c r="C150" t="str">
+        <v>https://puruliadj.in/files/download/id/2</v>
+      </c>
+      <c r="D150" t="str">
+        <v>(New Jhargram Jhumur)</v>
+      </c>
+      <c r="E150" t="str">
+        <v>Old Jhargram Jhumur Mp3 Songs</v>
+      </c>
+      <c r="F150" t="str">
+        <v>class</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
         <v xml:space="preserve">Pagol Hoye Gali Re Nilima Kundan Kumar New Purulia Song 2024.mp3 </v>
       </c>
-      <c r="B142" t="str">
+      <c r="B151" t="str">
         <v>https://puruliadj.in/download/1/pagol_hoye_gali_re_nilima_kundan_kumar_new_purulia_song_2024</v>
       </c>
-      <c r="C142" t="str">
+      <c r="C151" t="str">
         <v>https://puruliadj.in/files/download/id/1</v>
       </c>
-      <c r="D142" t="str">
-        <v>(New Purulia Songs)</v>
-      </c>
-      <c r="E142" t="str">
-        <v>New Purulia Mp3 Songs</v>
-      </c>
-      <c r="F142" t="str">
+      <c r="D151" t="str">
+        <v>(New Purulia Songs)</v>
+      </c>
+      <c r="E151" t="str">
+        <v>New Purulia Mp3 Songs</v>
+      </c>
+      <c r="F151" t="str">
         <v>class</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F142"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F151"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>